<commit_message>
First version of strategic model water quality calculation
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PARETO - dev\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD209554-100D-4951-A0B9-B17115EE6659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A281873C-FBDA-465B-B9FC-C78D5FCEECB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="58" activeTab="66" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="50" activeTab="57" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -21184,8 +21184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21203,7 +21203,7 @@
         <v>242</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -29391,7 +29391,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29574,7 +29574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA869B1E-00E6-4DCA-8F85-295EB0728F7B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add Units tab to toy case studies, update small case study to have proper units, update tests
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC1D157-7BAA-4E6F-833D-BE5677A19D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5ADAD-09E1-491B-A03F-F82E237197C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="13" activeTab="37" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-15105" yWindow="-16425" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="2" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -10400,8 +10400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AE0639-D41B-42DF-BE98-6917EE00552F}">
   <dimension ref="A1:AY12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10556,7 +10556,7 @@
         <v>290</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D8" s="82"/>
       <c r="E8" s="83"/>
@@ -11698,7 +11698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:BA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update all case study with correct unit tab, add process_constraint() to eliminate redundancy in checking that constraints are non empty
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E14B8D-AF44-455D-8F65-9EE7F53FB404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF27A505-14E4-4E6D-B002-6D788C50F559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="1" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="19080" yWindow="-15300" windowWidth="21600" windowHeight="12675" tabRatio="834" firstSheet="2" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>

</xml_diff>

<commit_message>
Add N19-N22 and N26-N28 nodes both ways in NNA tab
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE72104-0A69-4A98-99EF-AE949F6AE0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707000D-9AB0-477B-8E5A-0F574D927476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="8" activeTab="20" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2468,7 +2468,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5159,9 +5159,7 @@
   </sheetPr>
   <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6087,7 +6085,9 @@
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
+      <c r="T24" s="10">
+        <v>1</v>
+      </c>
       <c r="U24" s="10"/>
       <c r="V24" s="10">
         <v>1</v>
@@ -6322,7 +6322,9 @@
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
       <c r="Z30" s="10"/>
-      <c r="AA30" s="10"/>
+      <c r="AA30" s="10">
+        <v>1</v>
+      </c>
       <c r="AB30" s="10"/>
       <c r="AC30" s="10"/>
       <c r="AD30" s="32"/>

</xml_diff>

<commit_message>
Remove N10 - N12 arc in NNA tab
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707000D-9AB0-477B-8E5A-0F574D927476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734613A2-0011-4555-9E95-0B32D3E9127E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="8" activeTab="20" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="16" activeTab="20" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1663,7 +1663,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1923,6 +1923,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3270,9 +3271,7 @@
   </sheetPr>
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3298,7 +3297,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="111"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -5626,9 +5625,7 @@
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="10">
-        <v>1</v>
-      </c>
+      <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
@@ -5698,9 +5695,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10">
-        <v>1</v>
-      </c>
+      <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>

</xml_diff>

<commit_message>
Add N01 - K01 arc to NKA tab
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BAEE5C-8228-4576-89B4-8B319E07EDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DEBDCE-817C-4E3C-96AD-C3157DEE3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="19" activeTab="40" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="19" activeTab="22" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -6744,7 +6744,7 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6775,7 +6775,9 @@
       <c r="A3" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
       <c r="C3" s="10"/>
       <c r="D3" s="32"/>
     </row>
@@ -13633,7 +13635,7 @@
   </sheetPr>
   <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add limits for CP02-04 in PadOffloadingCapacity
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DEBDCE-817C-4E3C-96AD-C3157DEE3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0B8F28-951B-42EB-A806-6B6752D80256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="19" activeTab="22" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="38" activeTab="46" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -95,6 +95,7 @@
     <definedName name="_xlnm.Extract" localSheetId="63">PipelineExpansionDistance!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="287">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -6744,7 +6745,7 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17958,19 +17959,20 @@
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity  [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Pad Offloading Capacity  [bbl/week]</v>
+        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pad Offloading Capacity [bbl/week]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -17981,15 +17983,40 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="38">
         <v>210000</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="38">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="38">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="40">
+        <v>210000</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove nonzero entries from PipelineOperationalCost tab
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0B8F28-951B-42EB-A806-6B6752D80256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4FDF1C-8E37-4813-9E8A-49AAD76766BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="38" activeTab="46" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="45" activeTab="52" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="287">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -17961,7 +17961,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19178,141 +19178,36 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Pipeline Operational Cost between Sites [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="46">
-        <v>1E-4</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46">
-        <v>1E-4</v>
-      </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="46">
-        <v>1E-4</v>
-      </c>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="32">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="32"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="32"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="32"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="B2" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Add trucking hourly cost value for F03-F08
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4FDF1C-8E37-4813-9E8A-49AAD76766BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A56EDF-590B-44F0-8507-C95010ABB214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="45" activeTab="52" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="47" activeTab="54" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="287">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -1701,7 +1701,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1990,6 +1990,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -19180,7 +19183,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19319,9 +19322,9 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19455,10 +19458,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="122">
         <v>98</v>
       </c>
     </row>
@@ -19487,10 +19490,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="122">
         <v>95</v>
       </c>
     </row>
@@ -19502,11 +19505,59 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="12">
         <v>110</v>
       </c>
     </row>
@@ -19524,7 +19575,9 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19679,6 +19732,7 @@
       <c r="B20" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add trucking times for PP04-PP15
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A56EDF-590B-44F0-8507-C95010ABB214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86199824-DD3B-4511-ADAF-1A2CACB611D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="47" activeTab="54" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="47" activeTab="55" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3510" uniqueCount="287">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -1701,7 +1701,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1993,6 +1993,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -19324,7 +19327,7 @@
   </sheetPr>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19573,11 +19576,9 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19647,13 +19648,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
-        <v>3</v>
-      </c>
       <c r="C6" s="10">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="32">
         <v>6</v>
@@ -19661,13 +19662,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B7" s="10">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="C7" s="10">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="D7" s="32">
         <v>5</v>
@@ -19675,61 +19676,199 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="10">
+        <v>9</v>
+      </c>
+      <c r="C8" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="D8" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="10">
+        <v>8.5</v>
+      </c>
+      <c r="C9" s="10">
+        <v>9</v>
+      </c>
+      <c r="D9" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="10">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="10">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="D11" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="10">
+        <v>11.5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>12</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="10">
+        <v>12</v>
+      </c>
+      <c r="C13" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="D13" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="C14" s="10">
+        <v>13</v>
+      </c>
+      <c r="D14" s="32">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="C15" s="10">
+        <v>13</v>
+      </c>
+      <c r="D15" s="32">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="C16" s="10">
+        <v>13</v>
+      </c>
+      <c r="D16" s="32">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="123">
+        <v>11.5</v>
+      </c>
+      <c r="C17" s="123">
+        <v>12</v>
+      </c>
+      <c r="D17" s="122">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="10">
+        <v>3</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2</v>
+      </c>
+      <c r="D19" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B20" s="10">
         <v>8</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C20" s="10">
         <v>6</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D20" s="32">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B21" s="11">
         <v>8</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C21" s="11">
         <v>9</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D21" s="12">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Remove NSA and SNA arc between S01 and N12
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86199824-DD3B-4511-ADAF-1A2CACB611D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33A5A5F-8899-4B92-B522-465EB45F8AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="47" activeTab="55" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="10" activeTab="25" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -95,7 +95,6 @@
     <definedName name="_xlnm.Extract" localSheetId="63">PipelineExpansionDistance!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1701,7 +1700,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1998,6 +1997,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -7278,13 +7278,13 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7301,12 +7301,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
+      <c r="A3" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="124"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7321,13 +7319,12 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7340,16 +7337,14 @@
         <v>215</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
+      <c r="B3" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19578,7 +19573,9 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add some additional data about S02
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548E8CA-F441-4866-BECC-39B7A2204363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D43CC38-0AF5-4A0F-B571-74B129849EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="14" activeTab="27" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="66" activeTab="74" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3515" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3518" uniqueCount="288">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -1108,7 +1108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1376,36 +1376,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1697,7 +1667,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1796,9 +1766,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1845,10 +1812,10 @@
     <xf numFmtId="43" fontId="1" fillId="3" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1857,85 +1824,79 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1944,16 +1905,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1962,7 +1923,7 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1971,10 +1932,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1986,11 +1947,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3309,15 +3276,15 @@
       <c r="A3" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
+      <c r="A4" s="96"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
+      <c r="A5" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3358,7 +3325,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
+      <c r="A3" s="96"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -3988,7 +3955,7 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
+      <c r="A4" s="96"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -4067,7 +4034,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
+      <c r="A3" s="96"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4088,7 +4055,7 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
+      <c r="A4" s="96"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -7270,7 +7237,9 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7300,7 +7269,7 @@
         <v>130</v>
       </c>
       <c r="B3" s="33"/>
-      <c r="C3" s="121"/>
+      <c r="C3" s="118"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7479,7 +7448,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -7649,46 +7618,46 @@
       <c r="B2" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="83" t="s">
         <v>266</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="84" t="s">
         <v>267</v>
       </c>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="71"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="68"/>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="69" t="s">
         <v>268</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="74" t="s">
+      <c r="H3" s="72"/>
+      <c r="I3" s="71" t="s">
         <v>270</v>
       </c>
-      <c r="J3" s="73" t="s">
+      <c r="J3" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="73" t="s">
         <v>271</v>
       </c>
     </row>
@@ -7696,109 +7665,109 @@
       <c r="A4" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="54" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="69" t="s">
         <v>242</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="G4" s="74" t="s">
+      <c r="G4" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="76"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="76" t="s">
         <v>273</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="80"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="76" t="s">
         <v>274</v>
       </c>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="69" t="s">
         <v>247</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="H6" s="79"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="80"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="77"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="54" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="76" t="s">
         <v>275</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="69" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="G7" s="74" t="s">
+      <c r="G7" s="71" t="s">
         <v>252</v>
       </c>
-      <c r="H7" s="79"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="80"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="77"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="76" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="80"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="77"/>
       <c r="AT8" s="46" t="s">
         <v>237</v>
       </c>
@@ -7828,26 +7797,26 @@
       <c r="B9" s="39" t="s">
         <v>257</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="81" t="s">
         <v>277</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="78" t="s">
         <v>258</v>
       </c>
-      <c r="F9" s="82" t="s">
+      <c r="F9" s="79" t="s">
         <v>238</v>
       </c>
-      <c r="G9" s="83" t="s">
+      <c r="G9" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="H9" s="84"/>
-      <c r="I9" s="85" t="s">
+      <c r="H9" s="81"/>
+      <c r="I9" s="82" t="s">
         <v>260</v>
       </c>
-      <c r="J9" s="82" t="s">
+      <c r="J9" s="79" t="s">
         <v>238</v>
       </c>
-      <c r="K9" s="83" t="s">
+      <c r="K9" s="80" t="s">
         <v>261</v>
       </c>
       <c r="AT9" s="1" t="s">
@@ -7947,7 +7916,9 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8011,76 +7982,76 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
-      <c r="B5" s="122"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="122"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="122"/>
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
+      <c r="A6" s="119"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
+      <c r="A7" s="119"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
+      <c r="A8" s="119"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
+      <c r="A9" s="119"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
+      <c r="A10" s="119"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
+      <c r="A11" s="119"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="122"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
+      <c r="A12" s="119"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
-      <c r="B13" s="122"/>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122"/>
-      <c r="E13" s="122"/>
-      <c r="F13" s="122"/>
+      <c r="A13" s="119"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8875,7 +8846,9 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13736,7 +13709,9 @@
   </sheetPr>
   <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16364,13 +16339,15 @@
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
@@ -16389,12 +16366,20 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="39">
-        <v>0</v>
+      <c r="B3" s="37">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="39">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -16430,7 +16415,7 @@
       <c r="A2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="86" t="s">
         <v>278</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -16441,10 +16426,10 @@
       <c r="A3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="100">
+      <c r="B3" s="97">
         <v>75000</v>
       </c>
-      <c r="C3" s="90">
+      <c r="C3" s="87">
         <v>0</v>
       </c>
     </row>
@@ -16452,7 +16437,7 @@
       <c r="A4" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="101">
+      <c r="B4" s="98">
         <v>50000</v>
       </c>
       <c r="C4" s="39">
@@ -18201,324 +18186,324 @@
       </c>
     </row>
     <row r="2" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="110" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="113" t="s">
+      <c r="C2" s="110" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="110" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="113" t="s">
+      <c r="E2" s="110" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="110" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="113" t="s">
+      <c r="G2" s="110" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="113" t="s">
+      <c r="H2" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I2" s="113" t="s">
+      <c r="I2" s="110" t="s">
         <v>174</v>
       </c>
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="110" t="s">
         <v>175</v>
       </c>
-      <c r="K2" s="113" t="s">
+      <c r="K2" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="113" t="s">
+      <c r="L2" s="110" t="s">
         <v>155</v>
       </c>
-      <c r="M2" s="113" t="s">
+      <c r="M2" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="N2" s="113" t="s">
+      <c r="N2" s="110" t="s">
         <v>157</v>
       </c>
-      <c r="O2" s="113" t="s">
+      <c r="O2" s="110" t="s">
         <v>158</v>
       </c>
-      <c r="P2" s="113" t="s">
+      <c r="P2" s="110" t="s">
         <v>159</v>
       </c>
-      <c r="Q2" s="113" t="s">
+      <c r="Q2" s="110" t="s">
         <v>160</v>
       </c>
-      <c r="R2" s="113" t="s">
+      <c r="R2" s="110" t="s">
         <v>161</v>
       </c>
-      <c r="S2" s="113" t="s">
+      <c r="S2" s="110" t="s">
         <v>162</v>
       </c>
-      <c r="T2" s="113" t="s">
+      <c r="T2" s="110" t="s">
         <v>163</v>
       </c>
-      <c r="U2" s="113" t="s">
+      <c r="U2" s="110" t="s">
         <v>164</v>
       </c>
-      <c r="V2" s="113" t="s">
+      <c r="V2" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="W2" s="113" t="s">
+      <c r="W2" s="110" t="s">
         <v>166</v>
       </c>
-      <c r="X2" s="113" t="s">
+      <c r="X2" s="110" t="s">
         <v>178</v>
       </c>
-      <c r="Y2" s="113" t="s">
+      <c r="Y2" s="110" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="113" t="s">
+      <c r="Z2" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="AA2" s="113" t="s">
+      <c r="AA2" s="110" t="s">
         <v>181</v>
       </c>
-      <c r="AB2" s="113" t="s">
+      <c r="AB2" s="110" t="s">
         <v>182</v>
       </c>
-      <c r="AC2" s="113" t="s">
+      <c r="AC2" s="110" t="s">
         <v>183</v>
       </c>
-      <c r="AD2" s="113" t="s">
+      <c r="AD2" s="110" t="s">
         <v>184</v>
       </c>
-      <c r="AE2" s="113" t="s">
+      <c r="AE2" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="AF2" s="113" t="s">
+      <c r="AF2" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="AG2" s="113" t="s">
+      <c r="AG2" s="110" t="s">
         <v>187</v>
       </c>
-      <c r="AH2" s="113" t="s">
+      <c r="AH2" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="AI2" s="113" t="s">
+      <c r="AI2" s="110" t="s">
         <v>189</v>
       </c>
-      <c r="AJ2" s="113" t="s">
+      <c r="AJ2" s="110" t="s">
         <v>190</v>
       </c>
-      <c r="AK2" s="113" t="s">
+      <c r="AK2" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="AL2" s="113" t="s">
+      <c r="AL2" s="110" t="s">
         <v>192</v>
       </c>
-      <c r="AM2" s="113" t="s">
+      <c r="AM2" s="110" t="s">
         <v>193</v>
       </c>
-      <c r="AN2" s="113" t="s">
+      <c r="AN2" s="110" t="s">
         <v>194</v>
       </c>
-      <c r="AO2" s="113" t="s">
+      <c r="AO2" s="110" t="s">
         <v>195</v>
       </c>
-      <c r="AP2" s="113" t="s">
+      <c r="AP2" s="110" t="s">
         <v>196</v>
       </c>
-      <c r="AQ2" s="113" t="s">
+      <c r="AQ2" s="110" t="s">
         <v>197</v>
       </c>
-      <c r="AR2" s="113" t="s">
+      <c r="AR2" s="110" t="s">
         <v>198</v>
       </c>
-      <c r="AS2" s="113" t="s">
+      <c r="AS2" s="110" t="s">
         <v>199</v>
       </c>
-      <c r="AT2" s="113" t="s">
+      <c r="AT2" s="110" t="s">
         <v>200</v>
       </c>
-      <c r="AU2" s="113" t="s">
+      <c r="AU2" s="110" t="s">
         <v>201</v>
       </c>
-      <c r="AV2" s="113" t="s">
+      <c r="AV2" s="110" t="s">
         <v>202</v>
       </c>
-      <c r="AW2" s="113" t="s">
+      <c r="AW2" s="110" t="s">
         <v>203</v>
       </c>
-      <c r="AX2" s="113" t="s">
+      <c r="AX2" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="AY2" s="113" t="s">
+      <c r="AY2" s="110" t="s">
         <v>205</v>
       </c>
-      <c r="AZ2" s="113" t="s">
+      <c r="AZ2" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="BA2" s="114" t="s">
+      <c r="BA2" s="111" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="115">
-        <v>1</v>
-      </c>
-      <c r="D3" s="115">
-        <v>1</v>
-      </c>
-      <c r="E3" s="115">
-        <v>1</v>
-      </c>
-      <c r="F3" s="115">
-        <v>1</v>
-      </c>
-      <c r="G3" s="115">
-        <v>1</v>
-      </c>
-      <c r="H3" s="115">
-        <v>1</v>
-      </c>
-      <c r="I3" s="115">
-        <v>1</v>
-      </c>
-      <c r="J3" s="115">
-        <v>1</v>
-      </c>
-      <c r="K3" s="115">
-        <v>1</v>
-      </c>
-      <c r="L3" s="115">
-        <v>1</v>
-      </c>
-      <c r="M3" s="115">
-        <v>1</v>
-      </c>
-      <c r="N3" s="115">
-        <v>1</v>
-      </c>
-      <c r="O3" s="115">
-        <v>1</v>
-      </c>
-      <c r="P3" s="115">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="115">
-        <v>1</v>
-      </c>
-      <c r="R3" s="115">
-        <v>1</v>
-      </c>
-      <c r="S3" s="115">
-        <v>1</v>
-      </c>
-      <c r="T3" s="115">
-        <v>1</v>
-      </c>
-      <c r="U3" s="115">
-        <v>1</v>
-      </c>
-      <c r="V3" s="115">
-        <v>1</v>
-      </c>
-      <c r="W3" s="115">
-        <v>1</v>
-      </c>
-      <c r="X3" s="115">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="115">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AN3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AP3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AR3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AS3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AT3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AV3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AW3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AX3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AY3" s="115">
-        <v>1</v>
-      </c>
-      <c r="AZ3" s="115">
-        <v>1</v>
-      </c>
-      <c r="BA3" s="116">
+      <c r="B3" s="112">
+        <v>1</v>
+      </c>
+      <c r="C3" s="112">
+        <v>1</v>
+      </c>
+      <c r="D3" s="112">
+        <v>1</v>
+      </c>
+      <c r="E3" s="112">
+        <v>1</v>
+      </c>
+      <c r="F3" s="112">
+        <v>1</v>
+      </c>
+      <c r="G3" s="112">
+        <v>1</v>
+      </c>
+      <c r="H3" s="112">
+        <v>1</v>
+      </c>
+      <c r="I3" s="112">
+        <v>1</v>
+      </c>
+      <c r="J3" s="112">
+        <v>1</v>
+      </c>
+      <c r="K3" s="112">
+        <v>1</v>
+      </c>
+      <c r="L3" s="112">
+        <v>1</v>
+      </c>
+      <c r="M3" s="112">
+        <v>1</v>
+      </c>
+      <c r="N3" s="112">
+        <v>1</v>
+      </c>
+      <c r="O3" s="112">
+        <v>1</v>
+      </c>
+      <c r="P3" s="112">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="112">
+        <v>1</v>
+      </c>
+      <c r="R3" s="112">
+        <v>1</v>
+      </c>
+      <c r="S3" s="112">
+        <v>1</v>
+      </c>
+      <c r="T3" s="112">
+        <v>1</v>
+      </c>
+      <c r="U3" s="112">
+        <v>1</v>
+      </c>
+      <c r="V3" s="112">
+        <v>1</v>
+      </c>
+      <c r="W3" s="112">
+        <v>1</v>
+      </c>
+      <c r="X3" s="112">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="112">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="112">
+        <v>1</v>
+      </c>
+      <c r="AZ3" s="112">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="113">
         <v>1</v>
       </c>
     </row>
@@ -18843,16 +18828,16 @@
       <c r="BA5" s="11">
         <v>1</v>
       </c>
-      <c r="BD5" s="93"/>
+      <c r="BD5" s="90"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="B9" s="95"/>
+      <c r="B9" s="92"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F10" s="96"/>
+      <c r="F10" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19130,7 +19115,7 @@
       <c r="A2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="103" t="s">
         <v>281</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -19141,7 +19126,7 @@
       <c r="A3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="104" t="s">
         <v>278</v>
       </c>
       <c r="C3" s="34">
@@ -19152,7 +19137,7 @@
       <c r="A4" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="104" t="s">
         <v>278</v>
       </c>
       <c r="C4" s="34">
@@ -19163,7 +19148,7 @@
       <c r="A5" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="104" t="s">
         <v>279</v>
       </c>
       <c r="C5" s="34">
@@ -19174,32 +19159,32 @@
       <c r="A6" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="105" t="s">
         <v>279</v>
       </c>
       <c r="C6" s="35">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-    </row>
-    <row r="8" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-    </row>
-    <row r="9" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-    </row>
-    <row r="10" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
+    <row r="7" spans="1:3" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="95"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+    </row>
+    <row r="8" spans="1:3" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="95"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+    </row>
+    <row r="9" spans="1:3" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="95"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+    </row>
+    <row r="10" spans="1:3" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="95"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19555,10 +19540,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="119">
+      <c r="B17" s="116">
         <v>98</v>
       </c>
     </row>
@@ -19587,10 +19572,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="119">
+      <c r="B21" s="116">
         <v>95</v>
       </c>
     </row>
@@ -19897,16 +19882,16 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="120">
+      <c r="B17" s="117">
         <v>11.5</v>
       </c>
-      <c r="C17" s="120">
+      <c r="C17" s="117">
         <v>12</v>
       </c>
-      <c r="D17" s="119">
+      <c r="D17" s="116">
         <v>2.5</v>
       </c>
     </row>
@@ -20083,13 +20068,16 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20102,15 +20090,23 @@
       <c r="A2" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="120">
         <v>2</v>
       </c>
     </row>
@@ -20379,7 +20375,7 @@
       <c r="A2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="100" t="s">
         <v>281</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -20393,10 +20389,10 @@
       <c r="A3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="101" t="s">
         <v>278</v>
       </c>
-      <c r="C3" s="100">
+      <c r="C3" s="97">
         <v>10</v>
       </c>
       <c r="D3" s="37">
@@ -20407,10 +20403,10 @@
       <c r="A4" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="101" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="112">
+      <c r="C4" s="109">
         <v>10</v>
       </c>
       <c r="D4" s="37">
@@ -20421,10 +20417,10 @@
       <c r="A5" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="C5" s="112">
+      <c r="C5" s="109">
         <v>12</v>
       </c>
       <c r="D5" s="37">
@@ -20435,10 +20431,10 @@
       <c r="A6" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="102" t="s">
         <v>279</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="98">
         <v>12</v>
       </c>
       <c r="D6" s="39">
@@ -20581,7 +20577,9 @@
   </sheetPr>
   <dimension ref="A1:AN61"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView showZeros="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -20690,7 +20688,7 @@
       <c r="AF2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AG2" s="103" t="s">
+      <c r="AG2" s="100" t="s">
         <v>120</v>
       </c>
       <c r="AH2" s="7" t="s">
@@ -20812,7 +20810,7 @@
       <c r="AF3" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG3" s="117" t="s">
+      <c r="AG3" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH3" s="45" t="s">
@@ -20934,7 +20932,7 @@
       <c r="AF4" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG4" s="117" t="s">
+      <c r="AG4" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH4" s="45" t="s">
@@ -21056,7 +21054,7 @@
       <c r="AF5" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG5" s="117" t="s">
+      <c r="AG5" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH5" s="45" t="s">
@@ -21178,7 +21176,7 @@
       <c r="AF6" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG6" s="117" t="s">
+      <c r="AG6" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH6" s="45" t="s">
@@ -21300,7 +21298,7 @@
       <c r="AF7" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG7" s="117" t="s">
+      <c r="AG7" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH7" s="45" t="s">
@@ -21422,7 +21420,7 @@
       <c r="AF8" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG8" s="117" t="s">
+      <c r="AG8" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH8" s="45" t="s">
@@ -21544,7 +21542,7 @@
       <c r="AF9" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG9" s="117" t="s">
+      <c r="AG9" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH9" s="45" t="s">
@@ -21666,7 +21664,7 @@
       <c r="AF10" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG10" s="117" t="s">
+      <c r="AG10" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH10" s="45" t="s">
@@ -21788,7 +21786,7 @@
       <c r="AF11" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG11" s="117" t="s">
+      <c r="AG11" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH11" s="45" t="s">
@@ -21910,7 +21908,7 @@
       <c r="AF12" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG12" s="117" t="s">
+      <c r="AG12" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH12" s="45" t="s">
@@ -22032,7 +22030,7 @@
       <c r="AF13" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG13" s="117" t="s">
+      <c r="AG13" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH13" s="45" t="s">
@@ -22154,7 +22152,7 @@
       <c r="AF14" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG14" s="117" t="s">
+      <c r="AG14" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH14" s="45" t="s">
@@ -22276,7 +22274,7 @@
       <c r="AF15" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG15" s="117" t="s">
+      <c r="AG15" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH15" s="45" t="s">
@@ -22398,7 +22396,7 @@
       <c r="AF16" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG16" s="117" t="s">
+      <c r="AG16" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH16" s="45" t="s">
@@ -22520,7 +22518,7 @@
       <c r="AF17" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="AG17" s="118" t="s">
+      <c r="AG17" s="115" t="s">
         <v>235</v>
       </c>
       <c r="AH17" s="10" t="s">
@@ -22642,7 +22640,7 @@
       <c r="AF18" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="AG18" s="104" t="s">
+      <c r="AG18" s="101" t="s">
         <v>235</v>
       </c>
       <c r="AH18" s="45">
@@ -22764,7 +22762,7 @@
       <c r="AF19" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="AG19" s="104" t="s">
+      <c r="AG19" s="101" t="s">
         <v>235</v>
       </c>
       <c r="AH19" s="45">
@@ -22886,7 +22884,7 @@
       <c r="AF20" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="AG20" s="104" t="s">
+      <c r="AG20" s="101" t="s">
         <v>235</v>
       </c>
       <c r="AH20" s="45" t="s">
@@ -23008,7 +23006,7 @@
       <c r="AF21" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="AG21" s="105" t="s">
+      <c r="AG21" s="102" t="s">
         <v>235</v>
       </c>
       <c r="AH21" s="10" t="s">
@@ -23037,10 +23035,10 @@
       <c r="A22" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="52" t="s">
-        <v>235</v>
-      </c>
-      <c r="C22" s="52">
+      <c r="B22" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" s="51">
         <v>40.752409775985356</v>
       </c>
       <c r="D22" s="45" t="s">
@@ -23124,13 +23122,13 @@
       <c r="AD22" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="AE22" s="52">
+      <c r="AE22" s="51">
         <v>41.716999999999999</v>
       </c>
       <c r="AF22" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG22" s="117" t="s">
+      <c r="AG22" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH22" s="45" t="s">
@@ -23159,10 +23157,10 @@
       <c r="A23" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="52">
+      <c r="B23" s="51">
         <v>40.752409775985356</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="51" t="s">
         <v>235</v>
       </c>
       <c r="D23" s="45">
@@ -23252,7 +23250,7 @@
       <c r="AF23" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG23" s="117" t="s">
+      <c r="AG23" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH23" s="45" t="s">
@@ -23374,7 +23372,7 @@
       <c r="AF24" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG24" s="117" t="s">
+      <c r="AG24" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH24" s="45" t="s">
@@ -23496,7 +23494,7 @@
       <c r="AF25" s="45">
         <v>13.163</v>
       </c>
-      <c r="AG25" s="117" t="s">
+      <c r="AG25" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH25" s="45" t="s">
@@ -23528,7 +23526,7 @@
       <c r="B26" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="C26" s="52">
+      <c r="C26" s="51">
         <v>18.141999999999999</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -23618,7 +23616,7 @@
       <c r="AF26" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG26" s="117" t="s">
+      <c r="AG26" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH26" s="45" t="s">
@@ -23740,7 +23738,7 @@
       <c r="AF27" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG27" s="117" t="s">
+      <c r="AG27" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH27" s="45" t="s">
@@ -23862,7 +23860,7 @@
       <c r="AF28" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG28" s="117" t="s">
+      <c r="AG28" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH28" s="45" t="s">
@@ -23984,7 +23982,7 @@
       <c r="AF29" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG29" s="117" t="s">
+      <c r="AG29" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH29" s="45">
@@ -24106,7 +24104,7 @@
       <c r="AF30" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG30" s="117" t="s">
+      <c r="AG30" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH30" s="45" t="s">
@@ -24228,7 +24226,7 @@
       <c r="AF31" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG31" s="117" t="s">
+      <c r="AG31" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH31" s="45" t="s">
@@ -24350,7 +24348,7 @@
       <c r="AF32" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG32" s="117" t="s">
+      <c r="AG32" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH32" s="45" t="s">
@@ -24472,7 +24470,7 @@
       <c r="AF33" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG33" s="117" t="s">
+      <c r="AG33" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH33" s="45" t="s">
@@ -24594,7 +24592,7 @@
       <c r="AF34" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG34" s="117" t="s">
+      <c r="AG34" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH34" s="45" t="s">
@@ -24716,7 +24714,7 @@
       <c r="AF35" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG35" s="117" t="s">
+      <c r="AG35" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH35" s="45" t="s">
@@ -24838,7 +24836,7 @@
       <c r="AF36" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG36" s="117" t="s">
+      <c r="AG36" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH36" s="45" t="s">
@@ -24960,7 +24958,7 @@
       <c r="AF37" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG37" s="117" t="s">
+      <c r="AG37" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH37" s="45" t="s">
@@ -25082,7 +25080,7 @@
       <c r="AF38" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG38" s="117">
+      <c r="AG38" s="114">
         <v>64.859913942891041</v>
       </c>
       <c r="AH38" s="45" t="s">
@@ -25204,7 +25202,7 @@
       <c r="AF39" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG39" s="117">
+      <c r="AG39" s="114">
         <v>34.19</v>
       </c>
       <c r="AH39" s="45" t="s">
@@ -25326,7 +25324,7 @@
       <c r="AF40" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG40" s="117" t="s">
+      <c r="AG40" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH40" s="45" t="s">
@@ -25448,7 +25446,7 @@
       <c r="AF41" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG41" s="117" t="s">
+      <c r="AG41" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH41" s="45" t="s">
@@ -25570,7 +25568,7 @@
       <c r="AF42" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG42" s="117" t="s">
+      <c r="AG42" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH42" s="45" t="s">
@@ -25692,7 +25690,7 @@
       <c r="AF43" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG43" s="117" t="s">
+      <c r="AG43" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH43" s="45" t="s">
@@ -25814,7 +25812,7 @@
       <c r="AF44" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG44" s="117" t="s">
+      <c r="AG44" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH44" s="45" t="s">
@@ -25936,7 +25934,7 @@
       <c r="AF45" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG45" s="117" t="s">
+      <c r="AG45" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH45" s="45" t="s">
@@ -26058,7 +26056,7 @@
       <c r="AF46" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG46" s="117" t="s">
+      <c r="AG46" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH46" s="45" t="s">
@@ -26180,7 +26178,7 @@
       <c r="AF47" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG47" s="117" t="s">
+      <c r="AG47" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH47" s="45" t="s">
@@ -26302,7 +26300,7 @@
       <c r="AF48" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG48" s="117" t="s">
+      <c r="AG48" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH48" s="45" t="s">
@@ -26424,7 +26422,7 @@
       <c r="AF49" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG49" s="117" t="s">
+      <c r="AG49" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH49" s="45" t="s">
@@ -26546,7 +26544,7 @@
       <c r="AF50" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="AG50" s="118" t="s">
+      <c r="AG50" s="115" t="s">
         <v>235</v>
       </c>
       <c r="AH50" s="10" t="s">
@@ -26668,7 +26666,7 @@
       <c r="AF51" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="AG51" s="118" t="s">
+      <c r="AG51" s="115" t="s">
         <v>235</v>
       </c>
       <c r="AH51" s="10" t="s">
@@ -26790,7 +26788,7 @@
       <c r="AF52" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG52" s="117" t="s">
+      <c r="AG52" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH52" s="45" t="s">
@@ -26912,7 +26910,7 @@
       <c r="AF53" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG53" s="117" t="s">
+      <c r="AG53" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH53" s="45" t="s">
@@ -27034,7 +27032,7 @@
       <c r="AF54" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG54" s="117" t="s">
+      <c r="AG54" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH54" s="45" t="s">
@@ -27156,7 +27154,7 @@
       <c r="AF55" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG55" s="117" t="s">
+      <c r="AG55" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH55" s="45" t="s">
@@ -27278,7 +27276,7 @@
       <c r="AF56" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG56" s="117" t="s">
+      <c r="AG56" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH56" s="45" t="s">
@@ -27400,7 +27398,7 @@
       <c r="AF57" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG57" s="117" t="s">
+      <c r="AG57" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH57" s="45" t="s">
@@ -27522,7 +27520,7 @@
       <c r="AF58" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG58" s="117" t="s">
+      <c r="AG58" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH58" s="45" t="s">
@@ -27644,7 +27642,7 @@
       <c r="AF59" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="AG59" s="118" t="s">
+      <c r="AG59" s="115" t="s">
         <v>235</v>
       </c>
       <c r="AH59" s="10" t="s">
@@ -27766,7 +27764,7 @@
       <c r="AF60" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="AG60" s="117" t="s">
+      <c r="AG60" s="114" t="s">
         <v>235</v>
       </c>
       <c r="AH60" s="45" t="s">
@@ -27886,7 +27884,7 @@
       <c r="AF61" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="AG61" s="118" t="s">
+      <c r="AG61" s="115" t="s">
         <v>235</v>
       </c>
       <c r="AH61" s="10" t="s">
@@ -27938,10 +27936,10 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -27957,65 +27955,65 @@
       <c r="A3" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="49">
         <v>30</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="57"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="56"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="49">
         <v>30</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="57"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="56"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="49">
         <v>30</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="57"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="56"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="59">
         <v>30</v>
       </c>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28121,8 +28119,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28157,7 +28155,7 @@
       <c r="A2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="103" t="s">
         <v>281</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -28168,7 +28166,7 @@
       <c r="A3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="104" t="s">
         <v>278</v>
       </c>
       <c r="C3" s="34">
@@ -28179,7 +28177,7 @@
       <c r="A4" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="104" t="s">
         <v>278</v>
       </c>
       <c r="C4" s="34">
@@ -28190,7 +28188,7 @@
       <c r="A5" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="104" t="s">
         <v>279</v>
       </c>
       <c r="C5" s="34">
@@ -28201,7 +28199,7 @@
       <c r="A6" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="105" t="s">
         <v>279</v>
       </c>
       <c r="C6" s="35">
@@ -28209,24 +28207,24 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
+      <c r="A7" s="95"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
+      <c r="A8" s="95"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="98"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
+      <c r="A10" s="95"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28256,7 +28254,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="106" t="s">
         <v>281</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -28264,7 +28262,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="107" t="s">
         <v>278</v>
       </c>
       <c r="B3" s="37">
@@ -28272,7 +28270,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="108" t="s">
         <v>279</v>
       </c>
       <c r="B4" s="39">
@@ -28406,7 +28404,7 @@
       <c r="A2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="94" t="s">
         <v>211</v>
       </c>
     </row>
@@ -28414,7 +28412,7 @@
       <c r="A3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="92">
+      <c r="B3" s="89">
         <v>0</v>
       </c>
     </row>
@@ -28422,25 +28420,25 @@
       <c r="A4" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="94">
+      <c r="B4" s="91">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="98"/>
-      <c r="B5" s="98"/>
+      <c r="A5" s="95"/>
+      <c r="B5" s="95"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="98"/>
-      <c r="B6" s="98"/>
+      <c r="A6" s="95"/>
+      <c r="B6" s="95"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="95"/>
+      <c r="B7" s="95"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="95"/>
+      <c r="B8" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28466,7 +28464,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="88" t="s">
         <v>212</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -28490,10 +28488,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="53">
         <v>0</v>
       </c>
     </row>
@@ -28549,7 +28547,7 @@
       <c r="A4" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="50">
         <v>0.03</v>
       </c>
     </row>
@@ -28589,7 +28587,7 @@
       <c r="A3" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="54">
         <v>0.08</v>
       </c>
     </row>
@@ -28630,15 +28628,15 @@
       <c r="A2" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="64">
+      <c r="B3" s="63">
         <v>142277</v>
       </c>
     </row>
@@ -28646,7 +28644,7 @@
       <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="64">
         <v>140998</v>
       </c>
     </row>
@@ -28654,7 +28652,7 @@
       <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5" s="64">
         <v>172490.2</v>
       </c>
     </row>
@@ -28662,7 +28660,7 @@
       <c r="A6" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="65">
+      <c r="B6" s="64">
         <v>257547</v>
       </c>
     </row>
@@ -28670,7 +28668,7 @@
       <c r="A7" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="64">
         <v>241833.8</v>
       </c>
     </row>
@@ -28678,7 +28676,7 @@
       <c r="A8" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="65">
+      <c r="B8" s="64">
         <v>188503.7</v>
       </c>
     </row>
@@ -28686,7 +28684,7 @@
       <c r="A9" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="65">
+      <c r="B9" s="64">
         <v>146716</v>
       </c>
     </row>
@@ -28694,7 +28692,7 @@
       <c r="A10" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="65">
+      <c r="B10" s="64">
         <v>216563</v>
       </c>
     </row>
@@ -28702,7 +28700,7 @@
       <c r="A11" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="65">
+      <c r="B11" s="64">
         <v>150626</v>
       </c>
     </row>
@@ -28710,7 +28708,7 @@
       <c r="A12" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="65">
+      <c r="B12" s="64">
         <v>247061</v>
       </c>
     </row>
@@ -28718,7 +28716,7 @@
       <c r="A13" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="65">
+      <c r="B13" s="64">
         <v>180968</v>
       </c>
     </row>
@@ -28726,7 +28724,7 @@
       <c r="A14" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="65">
+      <c r="B14" s="64">
         <v>195584</v>
       </c>
     </row>
@@ -28734,7 +28732,7 @@
       <c r="A15" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="65">
+      <c r="B15" s="64">
         <v>148655</v>
       </c>
     </row>
@@ -28742,7 +28740,7 @@
       <c r="A16" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="65">
+      <c r="B16" s="64">
         <v>185369</v>
       </c>
     </row>
@@ -28750,7 +28748,7 @@
       <c r="A17" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="65">
+      <c r="B17" s="64">
         <v>222724</v>
       </c>
     </row>
@@ -28758,7 +28756,7 @@
       <c r="A18" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="64">
         <v>165376</v>
       </c>
     </row>
@@ -28766,7 +28764,7 @@
       <c r="A19" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="65">
+      <c r="B19" s="64">
         <v>240977</v>
       </c>
     </row>
@@ -28774,7 +28772,7 @@
       <c r="A20" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="65">
+      <c r="B20" s="64">
         <v>192794</v>
       </c>
     </row>
@@ -28782,7 +28780,7 @@
       <c r="A21" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="66">
+      <c r="B21" s="65">
         <v>216769</v>
       </c>
     </row>
@@ -28797,9 +28795,11 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28816,15 +28816,23 @@
       <c r="A2" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="67" t="s">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="68">
+      <c r="B3" s="63">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="65">
         <v>150000</v>
       </c>
     </row>
@@ -28857,7 +28865,7 @@
       <c r="A2" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>234</v>
       </c>
     </row>
@@ -28865,7 +28873,7 @@
       <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="65">
+      <c r="B3" s="64">
         <v>150000</v>
       </c>
     </row>
@@ -28873,7 +28881,7 @@
       <c r="A4" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="64">
         <v>150000</v>
       </c>
     </row>
@@ -28881,7 +28889,7 @@
       <c r="A5" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5" s="64">
         <v>150000</v>
       </c>
     </row>
@@ -28889,7 +28897,7 @@
       <c r="A6" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="66">
+      <c r="B6" s="65">
         <v>150000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unneeded RSA arcs
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D43CC38-0AF5-4A0F-B571-74B129849EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E837EB5-79F2-4868-A217-1F0ECF4F19A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="66" activeTab="74" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="16" activeTab="28" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -7519,8 +7519,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7553,17 +7553,13 @@
       <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="31">
-        <v>1</v>
-      </c>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
+      <c r="B4" s="10"/>
       <c r="C4" s="11">
         <v>1</v>
       </c>
@@ -7917,7 +7913,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8847,7 +8843,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -28797,7 +28793,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove RCA arcs, adjust initial pipeline capacity to ensure feasibility
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C3D79-16B5-46C6-B1FA-2C40CAD599B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD92867-D547-4AF2-A1B8-CDBCF3FF65C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="57" activeTab="63" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="27" activeTab="29" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1082,7 +1082,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1104,6 +1104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1667,7 +1673,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1956,6 +1962,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7484,12 +7496,8 @@
       <c r="A3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="31"/>
     </row>
@@ -7499,12 +7507,8 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11">
-        <v>1</v>
-      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7912,7 +7916,7 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -13706,12 +13710,16 @@
   <dimension ref="A1:AO57"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="1"/>
+    <col min="2" max="5" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="34" width="9.28515625" style="1"/>
+    <col min="35" max="38" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13924,10 +13932,14 @@
       <c r="AF3" s="36"/>
       <c r="AG3" s="36"/>
       <c r="AH3" s="36"/>
-      <c r="AI3" s="36"/>
-      <c r="AJ3" s="36"/>
-      <c r="AK3" s="36"/>
-      <c r="AL3" s="36"/>
+      <c r="AI3" s="122"/>
+      <c r="AJ3" s="122"/>
+      <c r="AK3" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="AL3" s="122">
+        <v>1000000</v>
+      </c>
       <c r="AM3" s="36">
         <v>100000</v>
       </c>
@@ -13973,12 +13985,14 @@
       <c r="AF4" s="36"/>
       <c r="AG4" s="36"/>
       <c r="AH4" s="36"/>
-      <c r="AI4" s="36"/>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="36">
-        <v>150000</v>
-      </c>
-      <c r="AL4" s="36"/>
+      <c r="AI4" s="122"/>
+      <c r="AJ4" s="122"/>
+      <c r="AK4" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="AL4" s="122">
+        <v>1000000</v>
+      </c>
       <c r="AM4" s="36"/>
       <c r="AN4" s="36"/>
       <c r="AO4" s="37"/>
@@ -14022,12 +14036,14 @@
       <c r="AF5" s="36"/>
       <c r="AG5" s="36"/>
       <c r="AH5" s="36"/>
-      <c r="AI5" s="36"/>
-      <c r="AJ5" s="36"/>
-      <c r="AK5" s="36">
-        <v>150000</v>
-      </c>
-      <c r="AL5" s="36"/>
+      <c r="AI5" s="122"/>
+      <c r="AJ5" s="122"/>
+      <c r="AK5" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="AL5" s="122">
+        <v>1000000</v>
+      </c>
       <c r="AM5" s="36"/>
       <c r="AN5" s="36"/>
       <c r="AO5" s="37"/>
@@ -14069,10 +14085,14 @@
       <c r="AF6" s="36"/>
       <c r="AG6" s="36"/>
       <c r="AH6" s="36"/>
-      <c r="AI6" s="36"/>
-      <c r="AJ6" s="36"/>
-      <c r="AK6" s="36"/>
-      <c r="AL6" s="36"/>
+      <c r="AI6" s="122"/>
+      <c r="AJ6" s="122"/>
+      <c r="AK6" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="AL6" s="122">
+        <v>1000000</v>
+      </c>
       <c r="AM6" s="36"/>
       <c r="AN6" s="36"/>
       <c r="AO6" s="37"/>
@@ -14081,14 +14101,10 @@
       <c r="A7" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="36">
-        <v>350000</v>
-      </c>
-      <c r="C7" s="36">
-        <v>300000</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="9"/>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
@@ -14120,10 +14136,10 @@
       <c r="AH7" s="36"/>
       <c r="AI7" s="36"/>
       <c r="AJ7" s="36"/>
-      <c r="AK7" s="36">
-        <v>300000</v>
-      </c>
-      <c r="AL7" s="36"/>
+      <c r="AK7" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="AL7" s="122"/>
       <c r="AM7" s="36"/>
       <c r="AN7" s="36"/>
       <c r="AO7" s="37"/>
@@ -14132,14 +14148,10 @@
       <c r="A8" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36">
-        <v>250000</v>
-      </c>
-      <c r="E8" s="36">
-        <v>300000</v>
-      </c>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
       <c r="F8" s="9"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
@@ -14171,8 +14183,10 @@
       <c r="AH8" s="36"/>
       <c r="AI8" s="36"/>
       <c r="AJ8" s="36"/>
-      <c r="AK8" s="36"/>
-      <c r="AL8" s="36"/>
+      <c r="AK8" s="122"/>
+      <c r="AL8" s="122">
+        <v>1000000</v>
+      </c>
       <c r="AM8" s="36"/>
       <c r="AN8" s="36"/>
       <c r="AO8" s="37"/>
@@ -16321,15 +16335,17 @@
       <c r="A53" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43">
-        <v>150000</v>
-      </c>
-      <c r="D53" s="43">
-        <v>150000</v>
-      </c>
-      <c r="E53" s="43">
-        <v>300000</v>
+      <c r="B53" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="C53" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="D53" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="E53" s="122">
+        <v>1000000</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="43"/>
@@ -16362,8 +16378,10 @@
       <c r="AF53" s="43"/>
       <c r="AG53" s="43"/>
       <c r="AH53" s="43"/>
-      <c r="AI53" s="43"/>
-      <c r="AJ53" s="43"/>
+      <c r="AI53" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="AJ53" s="123"/>
       <c r="AK53" s="43"/>
       <c r="AL53" s="43"/>
       <c r="AM53" s="43"/>
@@ -16374,10 +16392,18 @@
       <c r="A54" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
+      <c r="B54" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="C54" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="D54" s="122">
+        <v>1000000</v>
+      </c>
+      <c r="E54" s="122">
+        <v>1000000</v>
+      </c>
       <c r="F54" s="9"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
@@ -16407,8 +16433,10 @@
       <c r="AF54" s="43"/>
       <c r="AG54" s="43"/>
       <c r="AH54" s="43"/>
-      <c r="AI54" s="43"/>
-      <c r="AJ54" s="43"/>
+      <c r="AI54" s="123"/>
+      <c r="AJ54" s="122">
+        <v>1000000</v>
+      </c>
       <c r="AK54" s="43"/>
       <c r="AL54" s="43"/>
       <c r="AM54" s="43"/>
@@ -20863,7 +20891,7 @@
   </sheetPr>
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showZeros="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Remove unwanted SCA arcs, increase K02 disposal capacity to ensure feasibility of model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD92867-D547-4AF2-A1B8-CDBCF3FF65C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F447215E-8A40-4C37-A711-22C591138AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="27" activeTab="29" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="27" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -7916,7 +7916,7 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -7957,23 +7957,15 @@
       <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="31">
-        <v>1</v>
-      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="10">
         <v>1</v>
       </c>
@@ -13710,7 +13702,7 @@
   <dimension ref="A1:AO57"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16596,7 +16588,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16631,7 +16623,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="37">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adjust initial pipeline capacity values
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F447215E-8A40-4C37-A711-22C591138AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0E4788-1CC3-47C5-A86F-17651075A6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="27" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="66" activeTab="74" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1082,7 +1082,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1104,12 +1104,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1673,7 +1667,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1962,12 +1956,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7524,7 +7512,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7917,7 +7905,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8839,7 +8827,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13701,8 +13689,8 @@
   </sheetPr>
   <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13924,14 +13912,12 @@
       <c r="AF3" s="36"/>
       <c r="AG3" s="36"/>
       <c r="AH3" s="36"/>
-      <c r="AI3" s="122"/>
-      <c r="AJ3" s="122"/>
-      <c r="AK3" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="AL3" s="122">
-        <v>1000000</v>
-      </c>
+      <c r="AI3" s="36"/>
+      <c r="AJ3" s="36"/>
+      <c r="AK3" s="36">
+        <v>150000</v>
+      </c>
+      <c r="AL3" s="36"/>
       <c r="AM3" s="36">
         <v>100000</v>
       </c>
@@ -13977,14 +13963,12 @@
       <c r="AF4" s="36"/>
       <c r="AG4" s="36"/>
       <c r="AH4" s="36"/>
-      <c r="AI4" s="122"/>
-      <c r="AJ4" s="122"/>
-      <c r="AK4" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="AL4" s="122">
-        <v>1000000</v>
-      </c>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36">
+        <v>150000</v>
+      </c>
+      <c r="AL4" s="36"/>
       <c r="AM4" s="36"/>
       <c r="AN4" s="36"/>
       <c r="AO4" s="37"/>
@@ -14028,13 +14012,11 @@
       <c r="AF5" s="36"/>
       <c r="AG5" s="36"/>
       <c r="AH5" s="36"/>
-      <c r="AI5" s="122"/>
-      <c r="AJ5" s="122"/>
-      <c r="AK5" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="AL5" s="122">
-        <v>1000000</v>
+      <c r="AI5" s="36"/>
+      <c r="AJ5" s="36"/>
+      <c r="AK5" s="36"/>
+      <c r="AL5" s="36">
+        <v>150000</v>
       </c>
       <c r="AM5" s="36"/>
       <c r="AN5" s="36"/>
@@ -14077,13 +14059,11 @@
       <c r="AF6" s="36"/>
       <c r="AG6" s="36"/>
       <c r="AH6" s="36"/>
-      <c r="AI6" s="122"/>
-      <c r="AJ6" s="122"/>
-      <c r="AK6" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="AL6" s="122">
-        <v>1000000</v>
+      <c r="AI6" s="36"/>
+      <c r="AJ6" s="36"/>
+      <c r="AK6" s="36"/>
+      <c r="AL6" s="36">
+        <v>150000</v>
       </c>
       <c r="AM6" s="36"/>
       <c r="AN6" s="36"/>
@@ -14093,10 +14073,10 @@
       <c r="A7" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="9"/>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
@@ -14128,10 +14108,10 @@
       <c r="AH7" s="36"/>
       <c r="AI7" s="36"/>
       <c r="AJ7" s="36"/>
-      <c r="AK7" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="AL7" s="122"/>
+      <c r="AK7" s="36">
+        <v>300000</v>
+      </c>
+      <c r="AL7" s="36"/>
       <c r="AM7" s="36"/>
       <c r="AN7" s="36"/>
       <c r="AO7" s="37"/>
@@ -14140,10 +14120,10 @@
       <c r="A8" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="122"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="9"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
@@ -14175,9 +14155,9 @@
       <c r="AH8" s="36"/>
       <c r="AI8" s="36"/>
       <c r="AJ8" s="36"/>
-      <c r="AK8" s="122"/>
-      <c r="AL8" s="122">
-        <v>1000000</v>
+      <c r="AK8" s="36"/>
+      <c r="AL8" s="36">
+        <v>300000</v>
       </c>
       <c r="AM8" s="36"/>
       <c r="AN8" s="36"/>
@@ -14775,9 +14755,7 @@
       <c r="AH20" s="36"/>
       <c r="AI20" s="36"/>
       <c r="AJ20" s="36"/>
-      <c r="AK20" s="36">
-        <v>50000</v>
-      </c>
+      <c r="AK20" s="36"/>
       <c r="AL20" s="36"/>
       <c r="AM20" s="36"/>
       <c r="AN20" s="36"/>
@@ -16327,18 +16305,14 @@
       <c r="A53" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="C53" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="D53" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="E53" s="122">
-        <v>1000000</v>
-      </c>
+      <c r="B53" s="36">
+        <v>150000</v>
+      </c>
+      <c r="C53" s="36">
+        <v>150000</v>
+      </c>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
       <c r="F53" s="9"/>
       <c r="G53" s="43"/>
       <c r="H53" s="43"/>
@@ -16350,9 +16324,7 @@
       <c r="N53" s="43"/>
       <c r="O53" s="43"/>
       <c r="P53" s="43"/>
-      <c r="Q53" s="43">
-        <v>50000</v>
-      </c>
+      <c r="Q53" s="43"/>
       <c r="R53" s="43"/>
       <c r="S53" s="43"/>
       <c r="T53" s="43"/>
@@ -16370,10 +16342,10 @@
       <c r="AF53" s="43"/>
       <c r="AG53" s="43"/>
       <c r="AH53" s="43"/>
-      <c r="AI53" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="AJ53" s="123"/>
+      <c r="AI53" s="36">
+        <v>300000</v>
+      </c>
+      <c r="AJ53" s="43"/>
       <c r="AK53" s="43"/>
       <c r="AL53" s="43"/>
       <c r="AM53" s="43"/>
@@ -16384,17 +16356,13 @@
       <c r="A54" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="B54" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="C54" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="D54" s="122">
-        <v>1000000</v>
-      </c>
-      <c r="E54" s="122">
-        <v>1000000</v>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36">
+        <v>150000</v>
+      </c>
+      <c r="E54" s="36">
+        <v>150000</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="43"/>
@@ -16425,9 +16393,9 @@
       <c r="AF54" s="43"/>
       <c r="AG54" s="43"/>
       <c r="AH54" s="43"/>
-      <c r="AI54" s="123"/>
-      <c r="AJ54" s="122">
-        <v>1000000</v>
+      <c r="AI54" s="43"/>
+      <c r="AJ54" s="36">
+        <v>300000</v>
       </c>
       <c r="AK54" s="43"/>
       <c r="AL54" s="43"/>
@@ -16588,7 +16556,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20883,7 +20851,9 @@
   </sheetPr>
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showZeros="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -29208,8 +29178,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clean up InitialPipelineCapacity tab
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_strategic_case_study.xlsx
+++ b/pareto/case_studies/small_strategic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0E4788-1CC3-47C5-A86F-17651075A6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815DDBFD-B4FE-4C55-AF8C-39FC2E9AAA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="66" activeTab="74" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="40" activeTab="40" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1667,7 +1667,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1956,6 +1956,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5190,7 +5202,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13689,9 +13702,7 @@
   </sheetPr>
   <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13761,7 +13772,7 @@
       <c r="D2" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="100" t="s">
         <v>119</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -13848,19 +13859,19 @@
       <c r="AG2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="100" t="s">
         <v>151</v>
       </c>
       <c r="AI2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AJ2" s="7" t="s">
+      <c r="AJ2" s="100" t="s">
         <v>128</v>
       </c>
       <c r="AK2" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AL2" s="100" t="s">
         <v>287</v>
       </c>
       <c r="AM2" s="7" t="s">
@@ -13880,7 +13891,7 @@
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="E3" s="123"/>
       <c r="F3" s="9"/>
       <c r="G3" s="36"/>
       <c r="H3" s="36">
@@ -13911,16 +13922,14 @@
       <c r="AE3" s="36"/>
       <c r="AF3" s="36"/>
       <c r="AG3" s="36"/>
-      <c r="AH3" s="36"/>
+      <c r="AH3" s="123"/>
       <c r="AI3" s="36"/>
-      <c r="AJ3" s="36"/>
+      <c r="AJ3" s="123"/>
       <c r="AK3" s="36">
         <v>150000</v>
       </c>
-      <c r="AL3" s="36"/>
-      <c r="AM3" s="36">
-        <v>100000</v>
-      </c>
+      <c r="AL3" s="123"/>
+      <c r="AM3" s="36"/>
       <c r="AN3" s="36"/>
       <c r="AO3" s="37"/>
     </row>
@@ -13931,7 +13940,7 @@
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="E4" s="123"/>
       <c r="F4" s="9"/>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -13941,7 +13950,7 @@
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="43">
+      <c r="O4" s="36">
         <v>100000</v>
       </c>
       <c r="P4" s="36"/>
@@ -13962,13 +13971,13 @@
       <c r="AE4" s="36"/>
       <c r="AF4" s="36"/>
       <c r="AG4" s="36"/>
-      <c r="AH4" s="36"/>
+      <c r="AH4" s="123"/>
       <c r="AI4" s="36"/>
-      <c r="AJ4" s="36"/>
+      <c r="AJ4" s="123"/>
       <c r="AK4" s="36">
         <v>150000</v>
       </c>
-      <c r="AL4" s="36"/>
+      <c r="AL4" s="123"/>
       <c r="AM4" s="36"/>
       <c r="AN4" s="36"/>
       <c r="AO4" s="37"/>
@@ -13980,7 +13989,7 @@
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="E5" s="123"/>
       <c r="F5" s="9"/>
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
@@ -13997,7 +14006,7 @@
       <c r="S5" s="36"/>
       <c r="T5" s="36"/>
       <c r="U5" s="36"/>
-      <c r="V5" s="43">
+      <c r="V5" s="36">
         <v>150000</v>
       </c>
       <c r="W5" s="36"/>
@@ -14011,11 +14020,11 @@
       <c r="AE5" s="36"/>
       <c r="AF5" s="36"/>
       <c r="AG5" s="36"/>
-      <c r="AH5" s="36"/>
+      <c r="AH5" s="123"/>
       <c r="AI5" s="36"/>
-      <c r="AJ5" s="36"/>
+      <c r="AJ5" s="123"/>
       <c r="AK5" s="36"/>
-      <c r="AL5" s="36">
+      <c r="AL5" s="123">
         <v>150000</v>
       </c>
       <c r="AM5" s="36"/>
@@ -14023,62 +14032,64 @@
       <c r="AO5" s="37"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="36"/>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="36"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="36"/>
-      <c r="AB6" s="36"/>
-      <c r="AC6" s="36"/>
-      <c r="AD6" s="36"/>
-      <c r="AE6" s="36"/>
-      <c r="AF6" s="36"/>
-      <c r="AG6" s="36"/>
-      <c r="AH6" s="36"/>
-      <c r="AI6" s="36"/>
-      <c r="AJ6" s="36"/>
-      <c r="AK6" s="36"/>
-      <c r="AL6" s="36">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="122"/>
+      <c r="Q6" s="122"/>
+      <c r="R6" s="122"/>
+      <c r="S6" s="122"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="122"/>
+      <c r="V6" s="122"/>
+      <c r="W6" s="122"/>
+      <c r="X6" s="122"/>
+      <c r="Y6" s="122"/>
+      <c r="Z6" s="122"/>
+      <c r="AA6" s="122"/>
+      <c r="AB6" s="122"/>
+      <c r="AC6" s="122"/>
+      <c r="AD6" s="122"/>
+      <c r="AE6" s="122"/>
+      <c r="AF6" s="122"/>
+      <c r="AG6" s="122"/>
+      <c r="AH6" s="124"/>
+      <c r="AI6" s="122"/>
+      <c r="AJ6" s="124"/>
+      <c r="AK6" s="122"/>
+      <c r="AL6" s="124">
         <v>150000</v>
       </c>
-      <c r="AM6" s="36"/>
-      <c r="AN6" s="36"/>
-      <c r="AO6" s="37"/>
+      <c r="AM6" s="122"/>
+      <c r="AN6" s="122"/>
+      <c r="AO6" s="53"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
+      <c r="E7" s="123"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="36"/>
+      <c r="G7" s="36">
+        <v>50000</v>
+      </c>
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
@@ -14093,7 +14104,7 @@
       <c r="S7" s="36"/>
       <c r="T7" s="36"/>
       <c r="U7" s="36"/>
-      <c r="V7" s="43"/>
+      <c r="V7" s="36"/>
       <c r="W7" s="36"/>
       <c r="X7" s="36"/>
       <c r="Y7" s="36"/>
@@ -14105,30 +14116,36 @@
       <c r="AE7" s="36"/>
       <c r="AF7" s="36"/>
       <c r="AG7" s="36"/>
-      <c r="AH7" s="36"/>
+      <c r="AH7" s="123"/>
       <c r="AI7" s="36"/>
-      <c r="AJ7" s="36"/>
-      <c r="AK7" s="36">
-        <v>300000</v>
-      </c>
-      <c r="AL7" s="36"/>
-      <c r="AM7" s="36"/>
+      <c r="AJ7" s="123"/>
+      <c r="AK7" s="36"/>
+      <c r="AL7" s="123"/>
+      <c r="AM7" s="36">
+        <v>100000</v>
+      </c>
       <c r="AN7" s="36"/>
       <c r="AO7" s="37"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="36">
+        <v>50000</v>
+      </c>
       <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="H8" s="36">
+        <v>300000</v>
+      </c>
       <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
+      <c r="J8" s="36">
+        <v>300000</v>
+      </c>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -14140,7 +14157,7 @@
       <c r="S8" s="36"/>
       <c r="T8" s="36"/>
       <c r="U8" s="36"/>
-      <c r="V8" s="43"/>
+      <c r="V8" s="36"/>
       <c r="W8" s="36"/>
       <c r="X8" s="36"/>
       <c r="Y8" s="36"/>
@@ -14152,31 +14169,33 @@
       <c r="AE8" s="36"/>
       <c r="AF8" s="36"/>
       <c r="AG8" s="36"/>
-      <c r="AH8" s="36"/>
+      <c r="AH8" s="123"/>
       <c r="AI8" s="36"/>
-      <c r="AJ8" s="36"/>
+      <c r="AJ8" s="123"/>
       <c r="AK8" s="36"/>
-      <c r="AL8" s="36">
-        <v>300000</v>
-      </c>
+      <c r="AL8" s="123"/>
       <c r="AM8" s="36"/>
       <c r="AN8" s="36"/>
       <c r="AO8" s="37"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="B9" s="36">
+        <v>300000</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
+      <c r="E9" s="123"/>
       <c r="F9" s="9"/>
       <c r="G9" s="36">
-        <v>50000</v>
+        <v>300000</v>
       </c>
       <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
+      <c r="I9" s="36">
+        <v>300000</v>
+      </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
@@ -14189,7 +14208,7 @@
       <c r="S9" s="36"/>
       <c r="T9" s="36"/>
       <c r="U9" s="36"/>
-      <c r="V9" s="43"/>
+      <c r="V9" s="36"/>
       <c r="W9" s="36"/>
       <c r="X9" s="36"/>
       <c r="Y9" s="36"/>
@@ -14201,35 +14220,33 @@
       <c r="AE9" s="36"/>
       <c r="AF9" s="36"/>
       <c r="AG9" s="36"/>
-      <c r="AH9" s="36"/>
+      <c r="AH9" s="123"/>
       <c r="AI9" s="36"/>
-      <c r="AJ9" s="36"/>
+      <c r="AJ9" s="123"/>
       <c r="AK9" s="36"/>
-      <c r="AL9" s="36"/>
+      <c r="AL9" s="123"/>
       <c r="AM9" s="36"/>
       <c r="AN9" s="36"/>
       <c r="AO9" s="37"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="9">
-        <v>50000</v>
-      </c>
+      <c r="E10" s="123"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="36"/>
       <c r="H10" s="36">
         <v>300000</v>
       </c>
       <c r="I10" s="36"/>
-      <c r="J10" s="36">
+      <c r="J10" s="36"/>
+      <c r="K10" s="36">
         <v>300000</v>
       </c>
-      <c r="K10" s="36"/>
       <c r="L10" s="36"/>
       <c r="M10" s="36"/>
       <c r="N10" s="36"/>
@@ -14252,37 +14269,37 @@
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
       <c r="AG10" s="36"/>
-      <c r="AH10" s="36"/>
+      <c r="AH10" s="123"/>
       <c r="AI10" s="36"/>
-      <c r="AJ10" s="36"/>
+      <c r="AJ10" s="123"/>
       <c r="AK10" s="36"/>
-      <c r="AL10" s="36"/>
+      <c r="AL10" s="123"/>
       <c r="AM10" s="36"/>
-      <c r="AN10" s="36"/>
+      <c r="AN10" s="36">
+        <v>300000</v>
+      </c>
       <c r="AO10" s="37"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="36">
-        <v>300000</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B11" s="36"/>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
+      <c r="E11" s="123"/>
       <c r="F11" s="9"/>
       <c r="G11" s="36">
         <v>300000</v>
       </c>
       <c r="H11" s="36"/>
-      <c r="I11" s="36">
-        <v>300000</v>
-      </c>
+      <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
+      <c r="M11" s="36">
+        <v>300000</v>
+      </c>
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
       <c r="P11" s="36"/>
@@ -14303,34 +14320,34 @@
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
       <c r="AG11" s="36"/>
-      <c r="AH11" s="36"/>
+      <c r="AH11" s="123"/>
       <c r="AI11" s="36"/>
-      <c r="AJ11" s="36"/>
+      <c r="AJ11" s="123"/>
       <c r="AK11" s="36"/>
-      <c r="AL11" s="36"/>
+      <c r="AL11" s="123"/>
       <c r="AM11" s="36"/>
       <c r="AN11" s="36"/>
       <c r="AO11" s="37"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="E12" s="123"/>
       <c r="F12" s="9"/>
       <c r="G12" s="36"/>
-      <c r="H12" s="36">
+      <c r="H12" s="36"/>
+      <c r="I12" s="36">
         <v>300000</v>
       </c>
-      <c r="I12" s="36"/>
       <c r="J12" s="36"/>
-      <c r="K12" s="36">
+      <c r="K12" s="36"/>
+      <c r="L12" s="36">
         <v>300000</v>
       </c>
-      <c r="L12" s="36"/>
       <c r="M12" s="36"/>
       <c r="N12" s="36"/>
       <c r="O12" s="36"/>
@@ -14352,38 +14369,38 @@
       <c r="AE12" s="36"/>
       <c r="AF12" s="36"/>
       <c r="AG12" s="36"/>
-      <c r="AH12" s="36"/>
+      <c r="AH12" s="123"/>
       <c r="AI12" s="36"/>
-      <c r="AJ12" s="36"/>
+      <c r="AJ12" s="123"/>
       <c r="AK12" s="36"/>
-      <c r="AL12" s="36"/>
+      <c r="AL12" s="123"/>
       <c r="AM12" s="36"/>
-      <c r="AN12" s="36">
-        <v>300000</v>
-      </c>
+      <c r="AN12" s="36"/>
       <c r="AO12" s="37"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="E13" s="123"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="36">
-        <v>300000</v>
-      </c>
+      <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="36"/>
       <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
+      <c r="K13" s="36">
+        <v>300000</v>
+      </c>
       <c r="L13" s="36"/>
       <c r="M13" s="36">
         <v>300000</v>
       </c>
-      <c r="N13" s="36"/>
+      <c r="N13" s="36">
+        <v>250000</v>
+      </c>
       <c r="O13" s="36"/>
       <c r="P13" s="36"/>
       <c r="Q13" s="36"/>
@@ -14403,30 +14420,30 @@
       <c r="AE13" s="36"/>
       <c r="AF13" s="36"/>
       <c r="AG13" s="36"/>
-      <c r="AH13" s="36"/>
+      <c r="AH13" s="123"/>
       <c r="AI13" s="36"/>
-      <c r="AJ13" s="36"/>
+      <c r="AJ13" s="123"/>
       <c r="AK13" s="36"/>
-      <c r="AL13" s="36"/>
+      <c r="AL13" s="123"/>
       <c r="AM13" s="36"/>
       <c r="AN13" s="36"/>
       <c r="AO13" s="37"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="E14" s="123"/>
       <c r="F14" s="9"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
-      <c r="I14" s="36">
+      <c r="I14" s="36"/>
+      <c r="J14" s="36">
         <v>300000</v>
       </c>
-      <c r="J14" s="36"/>
       <c r="K14" s="36"/>
       <c r="L14" s="36">
         <v>300000</v>
@@ -14452,40 +14469,42 @@
       <c r="AE14" s="36"/>
       <c r="AF14" s="36"/>
       <c r="AG14" s="36"/>
-      <c r="AH14" s="36"/>
-      <c r="AI14" s="36"/>
-      <c r="AJ14" s="36"/>
+      <c r="AH14" s="123"/>
+      <c r="AI14" s="36">
+        <v>500000</v>
+      </c>
+      <c r="AJ14" s="123"/>
       <c r="AK14" s="36"/>
-      <c r="AL14" s="36"/>
+      <c r="AL14" s="123"/>
       <c r="AM14" s="36"/>
       <c r="AN14" s="36"/>
       <c r="AO14" s="37"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="E15" s="123"/>
       <c r="F15" s="9"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
-      <c r="K15" s="36">
-        <v>300000</v>
-      </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36">
-        <v>300000</v>
-      </c>
-      <c r="N15" s="36">
+      <c r="K15" s="36"/>
+      <c r="L15" s="36">
         <v>250000</v>
       </c>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36">
+        <v>200000</v>
+      </c>
+      <c r="P15" s="36">
+        <v>50000</v>
+      </c>
       <c r="Q15" s="36"/>
       <c r="R15" s="36"/>
       <c r="S15" s="36"/>
@@ -14503,36 +14522,36 @@
       <c r="AE15" s="36"/>
       <c r="AF15" s="36"/>
       <c r="AG15" s="36"/>
-      <c r="AH15" s="36"/>
+      <c r="AH15" s="123"/>
       <c r="AI15" s="36"/>
-      <c r="AJ15" s="36"/>
+      <c r="AJ15" s="123"/>
       <c r="AK15" s="36"/>
-      <c r="AL15" s="36"/>
+      <c r="AL15" s="123"/>
       <c r="AM15" s="36"/>
       <c r="AN15" s="36"/>
       <c r="AO15" s="37"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="C16" s="36">
+        <v>100000</v>
+      </c>
       <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="E16" s="123"/>
       <c r="F16" s="9"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
-      <c r="J16" s="36">
-        <v>300000</v>
-      </c>
+      <c r="J16" s="36"/>
       <c r="K16" s="36"/>
-      <c r="L16" s="36">
-        <v>300000</v>
-      </c>
+      <c r="L16" s="36"/>
       <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
+      <c r="N16" s="36">
+        <v>200000</v>
+      </c>
       <c r="O16" s="36"/>
       <c r="P16" s="36"/>
       <c r="Q16" s="36"/>
@@ -14552,44 +14571,40 @@
       <c r="AE16" s="36"/>
       <c r="AF16" s="36"/>
       <c r="AG16" s="36"/>
-      <c r="AH16" s="36"/>
-      <c r="AI16" s="36">
-        <v>500000</v>
-      </c>
-      <c r="AJ16" s="36"/>
+      <c r="AH16" s="123"/>
+      <c r="AI16" s="36"/>
+      <c r="AJ16" s="123"/>
       <c r="AK16" s="36"/>
-      <c r="AL16" s="36"/>
+      <c r="AL16" s="123"/>
       <c r="AM16" s="36"/>
       <c r="AN16" s="36"/>
       <c r="AO16" s="37"/>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B17" s="36"/>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
+      <c r="E17" s="123"/>
       <c r="F17" s="9"/>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
       <c r="I17" s="36"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
-      <c r="L17" s="36">
-        <v>250000</v>
-      </c>
+      <c r="L17" s="36"/>
       <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36">
-        <v>200000</v>
-      </c>
-      <c r="P17" s="36">
+      <c r="N17" s="36">
         <v>50000</v>
       </c>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
       <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
+      <c r="R17" s="36">
+        <v>50000</v>
+      </c>
       <c r="S17" s="36"/>
       <c r="T17" s="36"/>
       <c r="U17" s="36"/>
@@ -14605,23 +14620,23 @@
       <c r="AE17" s="36"/>
       <c r="AF17" s="36"/>
       <c r="AG17" s="36"/>
-      <c r="AH17" s="36"/>
+      <c r="AH17" s="123"/>
       <c r="AI17" s="36"/>
-      <c r="AJ17" s="36"/>
+      <c r="AJ17" s="123"/>
       <c r="AK17" s="36"/>
-      <c r="AL17" s="36"/>
+      <c r="AL17" s="123"/>
       <c r="AM17" s="36"/>
       <c r="AN17" s="36"/>
       <c r="AO17" s="37"/>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="123"/>
       <c r="F18" s="9"/>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>
@@ -14630,16 +14645,14 @@
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="36"/>
-      <c r="N18" s="36">
-        <v>200000</v>
-      </c>
+      <c r="N18" s="36"/>
       <c r="O18" s="36"/>
       <c r="P18" s="36"/>
-      <c r="Q18" s="36">
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36">
         <v>150000</v>
       </c>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
       <c r="T18" s="36"/>
       <c r="U18" s="36"/>
       <c r="V18" s="36"/>
@@ -14654,23 +14667,23 @@
       <c r="AE18" s="36"/>
       <c r="AF18" s="36"/>
       <c r="AG18" s="36"/>
-      <c r="AH18" s="36"/>
+      <c r="AH18" s="123"/>
       <c r="AI18" s="36"/>
-      <c r="AJ18" s="36"/>
+      <c r="AJ18" s="123"/>
       <c r="AK18" s="36"/>
-      <c r="AL18" s="36"/>
+      <c r="AL18" s="123"/>
       <c r="AM18" s="36"/>
       <c r="AN18" s="36"/>
       <c r="AO18" s="37"/>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
       <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
+      <c r="E19" s="123"/>
       <c r="F19" s="9"/>
       <c r="G19" s="36"/>
       <c r="H19" s="36"/>
@@ -14679,16 +14692,16 @@
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
-      <c r="N19" s="36">
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36">
         <v>50000</v>
       </c>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
       <c r="Q19" s="36"/>
-      <c r="R19" s="36">
+      <c r="R19" s="36"/>
+      <c r="S19" s="36">
         <v>50000</v>
       </c>
-      <c r="S19" s="36"/>
       <c r="T19" s="36"/>
       <c r="U19" s="36"/>
       <c r="V19" s="36"/>
@@ -14703,23 +14716,23 @@
       <c r="AE19" s="36"/>
       <c r="AF19" s="36"/>
       <c r="AG19" s="36"/>
-      <c r="AH19" s="36"/>
+      <c r="AH19" s="123"/>
       <c r="AI19" s="36"/>
-      <c r="AJ19" s="36"/>
+      <c r="AJ19" s="123"/>
       <c r="AK19" s="36"/>
-      <c r="AL19" s="36"/>
+      <c r="AL19" s="123"/>
       <c r="AM19" s="36"/>
       <c r="AN19" s="36"/>
       <c r="AO19" s="37"/>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
+      <c r="E20" s="123"/>
       <c r="F20" s="9"/>
       <c r="G20" s="36"/>
       <c r="H20" s="36"/>
@@ -14729,15 +14742,15 @@
       <c r="L20" s="36"/>
       <c r="M20" s="36"/>
       <c r="N20" s="36"/>
-      <c r="O20" s="36">
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36">
         <v>150000</v>
       </c>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36">
-        <v>150000</v>
-      </c>
+      <c r="R20" s="36">
+        <v>50000</v>
+      </c>
+      <c r="S20" s="36"/>
       <c r="T20" s="36"/>
       <c r="U20" s="36"/>
       <c r="V20" s="36"/>
@@ -14752,23 +14765,25 @@
       <c r="AE20" s="36"/>
       <c r="AF20" s="36"/>
       <c r="AG20" s="36"/>
-      <c r="AH20" s="36"/>
+      <c r="AH20" s="123">
+        <v>200000</v>
+      </c>
       <c r="AI20" s="36"/>
-      <c r="AJ20" s="36"/>
+      <c r="AJ20" s="123"/>
       <c r="AK20" s="36"/>
-      <c r="AL20" s="36"/>
+      <c r="AL20" s="123"/>
       <c r="AM20" s="36"/>
       <c r="AN20" s="36"/>
       <c r="AO20" s="37"/>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
+      <c r="E21" s="123"/>
       <c r="F21" s="9"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36"/>
@@ -14779,16 +14794,14 @@
       <c r="M21" s="36"/>
       <c r="N21" s="36"/>
       <c r="O21" s="36"/>
-      <c r="P21" s="36">
-        <v>50000</v>
-      </c>
+      <c r="P21" s="36"/>
       <c r="Q21" s="36"/>
       <c r="R21" s="36"/>
-      <c r="S21" s="36">
-        <v>50000</v>
-      </c>
+      <c r="S21" s="36"/>
       <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
+      <c r="U21" s="36">
+        <v>300000</v>
+      </c>
       <c r="V21" s="36"/>
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
@@ -14801,23 +14814,25 @@
       <c r="AE21" s="36"/>
       <c r="AF21" s="36"/>
       <c r="AG21" s="36"/>
-      <c r="AH21" s="36"/>
+      <c r="AH21" s="123">
+        <v>300000</v>
+      </c>
       <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
+      <c r="AJ21" s="123"/>
       <c r="AK21" s="36"/>
-      <c r="AL21" s="36"/>
+      <c r="AL21" s="123"/>
       <c r="AM21" s="36"/>
       <c r="AN21" s="36"/>
       <c r="AO21" s="37"/>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
+      <c r="E22" s="123"/>
       <c r="F22" s="9"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
@@ -14829,16 +14844,16 @@
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
       <c r="P22" s="36"/>
-      <c r="Q22" s="36">
-        <v>150000</v>
-      </c>
-      <c r="R22" s="36">
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36">
+        <v>300000</v>
+      </c>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36">
         <v>50000</v>
       </c>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
       <c r="Y22" s="36"/>
@@ -14850,761 +14865,765 @@
       <c r="AE22" s="36"/>
       <c r="AF22" s="36"/>
       <c r="AG22" s="36"/>
-      <c r="AH22" s="36">
-        <v>200000</v>
-      </c>
+      <c r="AH22" s="123"/>
       <c r="AI22" s="36"/>
-      <c r="AJ22" s="36"/>
+      <c r="AJ22" s="123"/>
       <c r="AK22" s="36"/>
-      <c r="AL22" s="36"/>
+      <c r="AL22" s="123"/>
       <c r="AM22" s="36"/>
       <c r="AN22" s="36"/>
       <c r="AO22" s="37"/>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+        <v>139</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36">
+        <v>150000</v>
+      </c>
+      <c r="E23" s="123"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="43">
-        <v>300000</v>
-      </c>
-      <c r="V23" s="43"/>
-      <c r="W23" s="43"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="43"/>
-      <c r="AB23" s="43"/>
-      <c r="AC23" s="43"/>
-      <c r="AD23" s="43"/>
-      <c r="AE23" s="43"/>
-      <c r="AF23" s="43"/>
-      <c r="AG23" s="43"/>
-      <c r="AH23" s="43">
-        <v>300000</v>
-      </c>
-      <c r="AI23" s="43"/>
-      <c r="AJ23" s="43"/>
-      <c r="AK23" s="43"/>
-      <c r="AL23" s="43"/>
-      <c r="AM23" s="43"/>
-      <c r="AN23" s="43"/>
-      <c r="AO23" s="37"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="36"/>
+      <c r="U23" s="36">
+        <v>50000</v>
+      </c>
+      <c r="V23" s="36"/>
+      <c r="W23" s="36"/>
+      <c r="X23" s="36"/>
+      <c r="Y23" s="36"/>
+      <c r="Z23" s="36"/>
+      <c r="AA23" s="36"/>
+      <c r="AB23" s="36"/>
+      <c r="AC23" s="36"/>
+      <c r="AD23" s="36"/>
+      <c r="AE23" s="36"/>
+      <c r="AF23" s="36"/>
+      <c r="AG23" s="36"/>
+      <c r="AH23" s="123"/>
+      <c r="AI23" s="36"/>
+      <c r="AJ23" s="123"/>
+      <c r="AK23" s="36"/>
+      <c r="AL23" s="123"/>
+      <c r="AM23" s="36"/>
+      <c r="AN23" s="36"/>
+      <c r="AO23" s="37">
+        <v>100000</v>
+      </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+        <v>140</v>
+      </c>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="123"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="43">
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="36"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="36">
         <v>300000</v>
       </c>
-      <c r="U24" s="43"/>
-      <c r="V24" s="43">
-        <v>50000</v>
-      </c>
-      <c r="W24" s="43"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="43"/>
-      <c r="AB24" s="43"/>
-      <c r="AC24" s="43"/>
-      <c r="AD24" s="43"/>
-      <c r="AE24" s="43"/>
-      <c r="AF24" s="43"/>
-      <c r="AG24" s="43"/>
-      <c r="AH24" s="43"/>
-      <c r="AI24" s="43"/>
-      <c r="AJ24" s="43"/>
-      <c r="AK24" s="43"/>
-      <c r="AL24" s="43"/>
-      <c r="AM24" s="43"/>
-      <c r="AN24" s="43"/>
-      <c r="AO24" s="37"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
+      <c r="AA24" s="36"/>
+      <c r="AB24" s="36"/>
+      <c r="AC24" s="36"/>
+      <c r="AD24" s="36"/>
+      <c r="AE24" s="36"/>
+      <c r="AF24" s="36"/>
+      <c r="AG24" s="36"/>
+      <c r="AH24" s="123"/>
+      <c r="AI24" s="36"/>
+      <c r="AJ24" s="123"/>
+      <c r="AK24" s="36"/>
+      <c r="AL24" s="123"/>
+      <c r="AM24" s="36"/>
+      <c r="AN24" s="36"/>
+      <c r="AO24" s="37">
+        <v>300000</v>
+      </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+        <v>141</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="123"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43">
-        <v>50000</v>
-      </c>
-      <c r="V25" s="43"/>
-      <c r="W25" s="43"/>
-      <c r="X25" s="43"/>
-      <c r="Y25" s="43"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="43"/>
-      <c r="AB25" s="43"/>
-      <c r="AC25" s="43"/>
-      <c r="AD25" s="43"/>
-      <c r="AE25" s="43"/>
-      <c r="AF25" s="43"/>
-      <c r="AG25" s="43"/>
-      <c r="AH25" s="43"/>
-      <c r="AI25" s="43"/>
-      <c r="AJ25" s="43"/>
-      <c r="AK25" s="43"/>
-      <c r="AL25" s="43"/>
-      <c r="AM25" s="43"/>
-      <c r="AN25" s="43"/>
-      <c r="AO25" s="37">
-        <v>100000</v>
-      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="36"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="36">
+        <v>300000</v>
+      </c>
+      <c r="X25" s="36"/>
+      <c r="Y25" s="36"/>
+      <c r="Z25" s="36"/>
+      <c r="AA25" s="36">
+        <v>300000</v>
+      </c>
+      <c r="AB25" s="36"/>
+      <c r="AC25" s="36"/>
+      <c r="AD25" s="36"/>
+      <c r="AE25" s="36"/>
+      <c r="AF25" s="36"/>
+      <c r="AG25" s="36"/>
+      <c r="AH25" s="123"/>
+      <c r="AI25" s="36"/>
+      <c r="AJ25" s="123"/>
+      <c r="AK25" s="36"/>
+      <c r="AL25" s="123"/>
+      <c r="AM25" s="36"/>
+      <c r="AN25" s="36"/>
+      <c r="AO25" s="37"/>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+        <v>142</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="123"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="43"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="43">
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="36"/>
+      <c r="V26" s="36"/>
+      <c r="W26" s="36"/>
+      <c r="X26" s="36"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36">
         <v>300000</v>
       </c>
-      <c r="Y26" s="43"/>
-      <c r="Z26" s="43"/>
-      <c r="AA26" s="43"/>
-      <c r="AB26" s="43"/>
-      <c r="AC26" s="43"/>
-      <c r="AD26" s="43"/>
-      <c r="AE26" s="43"/>
-      <c r="AF26" s="43"/>
-      <c r="AG26" s="43"/>
-      <c r="AH26" s="43"/>
-      <c r="AI26" s="43"/>
-      <c r="AJ26" s="43"/>
-      <c r="AK26" s="43"/>
-      <c r="AL26" s="43"/>
-      <c r="AM26" s="43"/>
-      <c r="AN26" s="43"/>
-      <c r="AO26" s="37">
+      <c r="AA26" s="36"/>
+      <c r="AB26" s="36"/>
+      <c r="AC26" s="36"/>
+      <c r="AD26" s="36"/>
+      <c r="AE26" s="36"/>
+      <c r="AF26" s="36"/>
+      <c r="AG26" s="36"/>
+      <c r="AH26" s="123">
         <v>300000</v>
       </c>
+      <c r="AI26" s="36"/>
+      <c r="AJ26" s="123">
+        <v>500000</v>
+      </c>
+      <c r="AK26" s="36"/>
+      <c r="AL26" s="123"/>
+      <c r="AM26" s="36"/>
+      <c r="AN26" s="36"/>
+      <c r="AO26" s="37"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+        <v>143</v>
+      </c>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="123"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43">
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="36"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
+      <c r="X27" s="36"/>
+      <c r="Y27" s="36">
         <v>300000</v>
       </c>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="43"/>
-      <c r="Z27" s="43"/>
-      <c r="AA27" s="43">
+      <c r="Z27" s="36"/>
+      <c r="AA27" s="36">
         <v>300000</v>
       </c>
-      <c r="AB27" s="43"/>
-      <c r="AC27" s="43"/>
-      <c r="AD27" s="43"/>
-      <c r="AE27" s="43"/>
-      <c r="AF27" s="43"/>
-      <c r="AG27" s="43"/>
-      <c r="AH27" s="43"/>
-      <c r="AI27" s="43"/>
-      <c r="AJ27" s="43"/>
-      <c r="AK27" s="43"/>
-      <c r="AL27" s="43"/>
-      <c r="AM27" s="43"/>
-      <c r="AN27" s="43"/>
+      <c r="AB27" s="36"/>
+      <c r="AC27" s="36"/>
+      <c r="AD27" s="36"/>
+      <c r="AE27" s="36"/>
+      <c r="AF27" s="36"/>
+      <c r="AG27" s="36"/>
+      <c r="AH27" s="123"/>
+      <c r="AI27" s="36"/>
+      <c r="AJ27" s="123"/>
+      <c r="AK27" s="36"/>
+      <c r="AL27" s="123"/>
+      <c r="AM27" s="36"/>
+      <c r="AN27" s="36"/>
       <c r="AO27" s="37"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
+        <v>144</v>
+      </c>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="123"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="43"/>
-      <c r="U28" s="43"/>
-      <c r="V28" s="43"/>
-      <c r="W28" s="43"/>
-      <c r="X28" s="43"/>
-      <c r="Y28" s="43"/>
-      <c r="Z28" s="43">
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="36"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="36"/>
+      <c r="X28" s="36">
         <v>300000</v>
       </c>
-      <c r="AA28" s="43"/>
-      <c r="AB28" s="43"/>
-      <c r="AC28" s="43"/>
-      <c r="AD28" s="43"/>
-      <c r="AE28" s="43"/>
-      <c r="AF28" s="43"/>
-      <c r="AG28" s="43"/>
-      <c r="AH28" s="43">
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="36">
         <v>300000</v>
       </c>
-      <c r="AI28" s="43"/>
-      <c r="AJ28" s="43">
-        <v>500000</v>
-      </c>
-      <c r="AK28" s="43"/>
-      <c r="AL28" s="43"/>
-      <c r="AM28" s="43"/>
-      <c r="AN28" s="43"/>
+      <c r="AA28" s="36"/>
+      <c r="AB28" s="36">
+        <v>100000</v>
+      </c>
+      <c r="AC28" s="36"/>
+      <c r="AD28" s="36"/>
+      <c r="AE28" s="36"/>
+      <c r="AF28" s="36"/>
+      <c r="AG28" s="36"/>
+      <c r="AH28" s="123"/>
+      <c r="AI28" s="36"/>
+      <c r="AJ28" s="123"/>
+      <c r="AK28" s="36"/>
+      <c r="AL28" s="123"/>
+      <c r="AM28" s="36"/>
+      <c r="AN28" s="36"/>
       <c r="AO28" s="37"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
+        <v>145</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="123"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="43">
-        <v>300000</v>
-      </c>
-      <c r="Z29" s="43"/>
-      <c r="AA29" s="43">
-        <v>300000</v>
-      </c>
-      <c r="AB29" s="43"/>
-      <c r="AC29" s="43"/>
-      <c r="AD29" s="43"/>
-      <c r="AE29" s="43"/>
-      <c r="AF29" s="43"/>
-      <c r="AG29" s="43"/>
-      <c r="AH29" s="43"/>
-      <c r="AI29" s="43"/>
-      <c r="AJ29" s="43"/>
-      <c r="AK29" s="43"/>
-      <c r="AL29" s="43"/>
-      <c r="AM29" s="43"/>
-      <c r="AN29" s="43"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="36"/>
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+      <c r="AA29" s="36">
+        <v>100000</v>
+      </c>
+      <c r="AB29" s="36"/>
+      <c r="AC29" s="36">
+        <v>100000</v>
+      </c>
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+      <c r="AF29" s="36"/>
+      <c r="AG29" s="36"/>
+      <c r="AH29" s="123"/>
+      <c r="AI29" s="36"/>
+      <c r="AJ29" s="123"/>
+      <c r="AK29" s="36"/>
+      <c r="AL29" s="123"/>
+      <c r="AM29" s="36"/>
+      <c r="AN29" s="36"/>
       <c r="AO29" s="37"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
+        <v>146</v>
+      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="123"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="43">
-        <v>300000</v>
-      </c>
-      <c r="AA30" s="43"/>
-      <c r="AB30" s="43">
-        <v>300000</v>
-      </c>
-      <c r="AC30" s="43"/>
-      <c r="AD30" s="43"/>
-      <c r="AE30" s="43"/>
-      <c r="AF30" s="43"/>
-      <c r="AG30" s="43"/>
-      <c r="AH30" s="43"/>
-      <c r="AI30" s="43"/>
-      <c r="AJ30" s="43"/>
-      <c r="AK30" s="43"/>
-      <c r="AL30" s="43"/>
-      <c r="AM30" s="43"/>
-      <c r="AN30" s="43"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AA30" s="36"/>
+      <c r="AB30" s="36">
+        <v>100000</v>
+      </c>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36">
+        <v>100000</v>
+      </c>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="123"/>
+      <c r="AI30" s="36"/>
+      <c r="AJ30" s="123"/>
+      <c r="AK30" s="36"/>
+      <c r="AL30" s="123"/>
+      <c r="AM30" s="36"/>
+      <c r="AN30" s="36"/>
       <c r="AO30" s="37"/>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
+        <v>147</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="123"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="43"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="43"/>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="43"/>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="43">
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36">
         <v>100000</v>
       </c>
-      <c r="AB31" s="43"/>
-      <c r="AC31" s="43">
-        <v>100000</v>
-      </c>
-      <c r="AD31" s="43"/>
-      <c r="AE31" s="43"/>
-      <c r="AF31" s="43"/>
-      <c r="AG31" s="43"/>
-      <c r="AH31" s="43"/>
-      <c r="AI31" s="43"/>
-      <c r="AJ31" s="43"/>
-      <c r="AK31" s="43"/>
-      <c r="AL31" s="43"/>
-      <c r="AM31" s="43"/>
-      <c r="AN31" s="43"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AF31" s="36"/>
+      <c r="AG31" s="36"/>
+      <c r="AH31" s="123"/>
+      <c r="AI31" s="36"/>
+      <c r="AJ31" s="123"/>
+      <c r="AK31" s="36"/>
+      <c r="AL31" s="123"/>
+      <c r="AM31" s="36"/>
+      <c r="AN31" s="36"/>
       <c r="AO31" s="37"/>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
+        <v>148</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="123"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="43"/>
-      <c r="U32" s="43"/>
-      <c r="V32" s="43"/>
-      <c r="W32" s="43"/>
-      <c r="X32" s="43"/>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="43"/>
-      <c r="AA32" s="43"/>
-      <c r="AB32" s="43">
-        <v>100000</v>
-      </c>
-      <c r="AC32" s="43"/>
-      <c r="AD32" s="43">
-        <v>100000</v>
-      </c>
-      <c r="AE32" s="43"/>
-      <c r="AF32" s="43"/>
-      <c r="AG32" s="43"/>
-      <c r="AH32" s="43"/>
-      <c r="AI32" s="43"/>
-      <c r="AJ32" s="43"/>
-      <c r="AK32" s="43"/>
-      <c r="AL32" s="43"/>
-      <c r="AM32" s="43"/>
-      <c r="AN32" s="43"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
+      <c r="AA32" s="36"/>
+      <c r="AB32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AD32" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AE32" s="36"/>
+      <c r="AF32" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AG32" s="36"/>
+      <c r="AH32" s="123"/>
+      <c r="AI32" s="36"/>
+      <c r="AJ32" s="123"/>
+      <c r="AK32" s="36"/>
+      <c r="AL32" s="123"/>
+      <c r="AM32" s="36"/>
+      <c r="AN32" s="36"/>
       <c r="AO32" s="37"/>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
+        <v>149</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="123"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43"/>
-      <c r="S33" s="43"/>
-      <c r="T33" s="43"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="43"/>
-      <c r="W33" s="43"/>
-      <c r="X33" s="43"/>
-      <c r="Y33" s="43"/>
-      <c r="Z33" s="43"/>
-      <c r="AA33" s="43"/>
-      <c r="AB33" s="43"/>
-      <c r="AC33" s="43">
-        <v>100000</v>
-      </c>
-      <c r="AD33" s="43"/>
-      <c r="AE33" s="43">
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
+      <c r="AA33" s="36"/>
+      <c r="AB33" s="36"/>
+      <c r="AC33" s="36"/>
+      <c r="AD33" s="36"/>
+      <c r="AE33" s="36">
         <v>50000</v>
       </c>
-      <c r="AF33" s="43"/>
-      <c r="AG33" s="43"/>
-      <c r="AH33" s="43"/>
-      <c r="AI33" s="43"/>
-      <c r="AJ33" s="43"/>
-      <c r="AK33" s="43"/>
-      <c r="AL33" s="43"/>
-      <c r="AM33" s="43"/>
-      <c r="AN33" s="43"/>
+      <c r="AF33" s="36"/>
+      <c r="AG33" s="36"/>
+      <c r="AH33" s="123"/>
+      <c r="AI33" s="36"/>
+      <c r="AJ33" s="123"/>
+      <c r="AK33" s="36"/>
+      <c r="AL33" s="123"/>
+      <c r="AM33" s="36"/>
+      <c r="AN33" s="36"/>
       <c r="AO33" s="37"/>
     </row>
     <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
+        <v>150</v>
+      </c>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="123"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="43"/>
-      <c r="U34" s="43"/>
-      <c r="V34" s="43"/>
-      <c r="W34" s="43"/>
-      <c r="X34" s="43"/>
-      <c r="Y34" s="43"/>
-      <c r="Z34" s="43"/>
-      <c r="AA34" s="43"/>
-      <c r="AB34" s="43"/>
-      <c r="AC34" s="43"/>
-      <c r="AD34" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AE34" s="43"/>
-      <c r="AF34" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AG34" s="43"/>
-      <c r="AH34" s="43"/>
-      <c r="AI34" s="43"/>
-      <c r="AJ34" s="43"/>
-      <c r="AK34" s="43"/>
-      <c r="AL34" s="43"/>
-      <c r="AM34" s="43"/>
-      <c r="AN34" s="43"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="36"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
+      <c r="V34" s="36"/>
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
+      <c r="AA34" s="36"/>
+      <c r="AB34" s="36"/>
+      <c r="AC34" s="36"/>
+      <c r="AD34" s="36"/>
+      <c r="AE34" s="36"/>
+      <c r="AF34" s="36"/>
+      <c r="AG34" s="36"/>
+      <c r="AH34" s="123"/>
+      <c r="AI34" s="36"/>
+      <c r="AJ34" s="123"/>
+      <c r="AK34" s="36"/>
+      <c r="AL34" s="123"/>
+      <c r="AM34" s="36"/>
+      <c r="AN34" s="36"/>
       <c r="AO34" s="37"/>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="43"/>
-      <c r="T35" s="43"/>
-      <c r="U35" s="43"/>
-      <c r="V35" s="43"/>
-      <c r="W35" s="43"/>
-      <c r="X35" s="43"/>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="43"/>
-      <c r="AA35" s="43"/>
-      <c r="AB35" s="43"/>
-      <c r="AC35" s="43"/>
-      <c r="AD35" s="43"/>
-      <c r="AE35" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AF35" s="43"/>
-      <c r="AG35" s="43"/>
-      <c r="AH35" s="43"/>
-      <c r="AI35" s="43"/>
-      <c r="AJ35" s="43"/>
-      <c r="AK35" s="43"/>
-      <c r="AL35" s="43"/>
-      <c r="AM35" s="43"/>
-      <c r="AN35" s="43"/>
-      <c r="AO35" s="37"/>
+      <c r="A35" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="122"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="122"/>
+      <c r="I35" s="122"/>
+      <c r="J35" s="122"/>
+      <c r="K35" s="122"/>
+      <c r="L35" s="122"/>
+      <c r="M35" s="122"/>
+      <c r="N35" s="122"/>
+      <c r="O35" s="122"/>
+      <c r="P35" s="122"/>
+      <c r="Q35" s="122"/>
+      <c r="R35" s="122"/>
+      <c r="S35" s="122">
+        <v>200000</v>
+      </c>
+      <c r="T35" s="122">
+        <v>300000</v>
+      </c>
+      <c r="U35" s="122"/>
+      <c r="V35" s="122"/>
+      <c r="W35" s="122"/>
+      <c r="X35" s="122"/>
+      <c r="Y35" s="122">
+        <v>300000</v>
+      </c>
+      <c r="Z35" s="122"/>
+      <c r="AA35" s="122"/>
+      <c r="AB35" s="122"/>
+      <c r="AC35" s="122"/>
+      <c r="AD35" s="122"/>
+      <c r="AE35" s="122"/>
+      <c r="AF35" s="122"/>
+      <c r="AG35" s="122"/>
+      <c r="AH35" s="124"/>
+      <c r="AI35" s="122"/>
+      <c r="AJ35" s="124"/>
+      <c r="AK35" s="122"/>
+      <c r="AL35" s="124"/>
+      <c r="AM35" s="122"/>
+      <c r="AN35" s="122"/>
+      <c r="AO35" s="53"/>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
+        <v>79</v>
+      </c>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="123"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
-      <c r="P36" s="43"/>
-      <c r="Q36" s="43"/>
-      <c r="R36" s="43"/>
-      <c r="S36" s="43"/>
-      <c r="T36" s="43"/>
-      <c r="U36" s="43"/>
-      <c r="V36" s="43"/>
-      <c r="W36" s="43"/>
-      <c r="X36" s="43"/>
-      <c r="Y36" s="43"/>
-      <c r="Z36" s="43"/>
-      <c r="AA36" s="43"/>
-      <c r="AB36" s="43"/>
-      <c r="AC36" s="43"/>
-      <c r="AD36" s="43"/>
-      <c r="AE36" s="43"/>
-      <c r="AF36" s="43"/>
-      <c r="AG36" s="43"/>
-      <c r="AH36" s="43"/>
-      <c r="AI36" s="43"/>
-      <c r="AJ36" s="43"/>
-      <c r="AK36" s="43"/>
-      <c r="AL36" s="43"/>
-      <c r="AM36" s="43"/>
-      <c r="AN36" s="43"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36">
+        <v>500000</v>
+      </c>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="36"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="36"/>
+      <c r="X36" s="36"/>
+      <c r="Y36" s="36"/>
+      <c r="Z36" s="36"/>
+      <c r="AA36" s="36"/>
+      <c r="AB36" s="36"/>
+      <c r="AC36" s="36"/>
+      <c r="AD36" s="36"/>
+      <c r="AE36" s="36"/>
+      <c r="AF36" s="36"/>
+      <c r="AG36" s="36"/>
+      <c r="AH36" s="123"/>
+      <c r="AI36" s="36"/>
+      <c r="AJ36" s="123"/>
+      <c r="AK36" s="36">
+        <v>300000</v>
+      </c>
+      <c r="AL36" s="123"/>
+      <c r="AM36" s="36"/>
+      <c r="AN36" s="36"/>
       <c r="AO36" s="37"/>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
-      <c r="P37" s="43"/>
-      <c r="Q37" s="43"/>
-      <c r="R37" s="43"/>
-      <c r="S37" s="43">
-        <v>200000</v>
-      </c>
-      <c r="T37" s="43">
+      <c r="A37" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="122"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="122"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="122"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="122"/>
+      <c r="K37" s="122"/>
+      <c r="L37" s="122"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="122"/>
+      <c r="O37" s="122"/>
+      <c r="P37" s="122"/>
+      <c r="Q37" s="122"/>
+      <c r="R37" s="122"/>
+      <c r="S37" s="122"/>
+      <c r="T37" s="122"/>
+      <c r="U37" s="122"/>
+      <c r="V37" s="122"/>
+      <c r="W37" s="122"/>
+      <c r="X37" s="122"/>
+      <c r="Y37" s="122">
+        <v>500000</v>
+      </c>
+      <c r="Z37" s="122"/>
+      <c r="AA37" s="122"/>
+      <c r="AB37" s="122"/>
+      <c r="AC37" s="122"/>
+      <c r="AD37" s="122"/>
+      <c r="AE37" s="122"/>
+      <c r="AF37" s="122"/>
+      <c r="AG37" s="122"/>
+      <c r="AH37" s="124"/>
+      <c r="AI37" s="122"/>
+      <c r="AJ37" s="124"/>
+      <c r="AK37" s="122"/>
+      <c r="AL37" s="124">
         <v>300000</v>
       </c>
-      <c r="U37" s="43"/>
-      <c r="V37" s="43"/>
-      <c r="W37" s="43"/>
-      <c r="X37" s="43"/>
-      <c r="Y37" s="43">
-        <v>300000</v>
-      </c>
-      <c r="Z37" s="43"/>
-      <c r="AA37" s="43"/>
-      <c r="AB37" s="43"/>
-      <c r="AC37" s="43"/>
-      <c r="AD37" s="43"/>
-      <c r="AE37" s="43"/>
-      <c r="AF37" s="43"/>
-      <c r="AG37" s="43"/>
-      <c r="AH37" s="43"/>
-      <c r="AI37" s="43"/>
-      <c r="AJ37" s="43"/>
-      <c r="AK37" s="43"/>
-      <c r="AL37" s="43"/>
-      <c r="AM37" s="43"/>
-      <c r="AN37" s="43"/>
-      <c r="AO37" s="37"/>
+      <c r="AM37" s="122"/>
+      <c r="AN37" s="122"/>
+      <c r="AO37" s="53"/>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
+        <v>78</v>
+      </c>
+      <c r="B38" s="36">
+        <v>150000</v>
+      </c>
+      <c r="C38" s="36">
+        <v>150000</v>
+      </c>
       <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="9">
-        <v>50000</v>
-      </c>
+      <c r="E38" s="123"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
       <c r="I38" s="36"/>
@@ -15632,78 +15651,84 @@
       <c r="AE38" s="36"/>
       <c r="AF38" s="36"/>
       <c r="AG38" s="36"/>
-      <c r="AH38" s="36"/>
-      <c r="AI38" s="36"/>
-      <c r="AJ38" s="36"/>
+      <c r="AH38" s="123"/>
+      <c r="AI38" s="36">
+        <v>300000</v>
+      </c>
+      <c r="AJ38" s="123"/>
       <c r="AK38" s="36"/>
-      <c r="AL38" s="36"/>
+      <c r="AL38" s="123"/>
       <c r="AM38" s="36"/>
       <c r="AN38" s="36"/>
       <c r="AO38" s="37"/>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36">
-        <v>100000</v>
-      </c>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
-      <c r="AA39" s="36"/>
-      <c r="AB39" s="36"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-      <c r="AE39" s="36"/>
-      <c r="AF39" s="36"/>
-      <c r="AG39" s="36"/>
-      <c r="AH39" s="36"/>
-      <c r="AI39" s="36"/>
-      <c r="AJ39" s="36"/>
-      <c r="AK39" s="36"/>
-      <c r="AL39" s="36"/>
-      <c r="AM39" s="36"/>
-      <c r="AN39" s="36"/>
-      <c r="AO39" s="37"/>
+      <c r="A39" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="B39" s="122"/>
+      <c r="C39" s="122"/>
+      <c r="D39" s="122">
+        <v>150000</v>
+      </c>
+      <c r="E39" s="124">
+        <v>150000</v>
+      </c>
+      <c r="F39" s="117"/>
+      <c r="G39" s="122"/>
+      <c r="H39" s="122"/>
+      <c r="I39" s="122"/>
+      <c r="J39" s="122"/>
+      <c r="K39" s="122"/>
+      <c r="L39" s="122"/>
+      <c r="M39" s="122"/>
+      <c r="N39" s="122"/>
+      <c r="O39" s="122"/>
+      <c r="P39" s="122"/>
+      <c r="Q39" s="122"/>
+      <c r="R39" s="122"/>
+      <c r="S39" s="122"/>
+      <c r="T39" s="122"/>
+      <c r="U39" s="122"/>
+      <c r="V39" s="122"/>
+      <c r="W39" s="122"/>
+      <c r="X39" s="122"/>
+      <c r="Y39" s="122"/>
+      <c r="Z39" s="122"/>
+      <c r="AA39" s="122"/>
+      <c r="AB39" s="122"/>
+      <c r="AC39" s="122"/>
+      <c r="AD39" s="122"/>
+      <c r="AE39" s="122"/>
+      <c r="AF39" s="122"/>
+      <c r="AG39" s="122"/>
+      <c r="AH39" s="124"/>
+      <c r="AI39" s="122"/>
+      <c r="AJ39" s="124">
+        <v>300000</v>
+      </c>
+      <c r="AK39" s="122"/>
+      <c r="AL39" s="124"/>
+      <c r="AM39" s="122"/>
+      <c r="AN39" s="122"/>
+      <c r="AO39" s="53"/>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="B40" s="36"/>
       <c r="C40" s="36"/>
       <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="9"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="36">
+        <v>100000</v>
+      </c>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
       <c r="J40" s="36"/>
-      <c r="K40" s="36">
-        <v>75000</v>
-      </c>
+      <c r="K40" s="36"/>
       <c r="L40" s="36"/>
       <c r="M40" s="36"/>
       <c r="N40" s="36"/>
@@ -15726,36 +15751,36 @@
       <c r="AE40" s="36"/>
       <c r="AF40" s="36"/>
       <c r="AG40" s="36"/>
-      <c r="AH40" s="36"/>
+      <c r="AH40" s="123"/>
       <c r="AI40" s="36"/>
-      <c r="AJ40" s="36"/>
+      <c r="AJ40" s="123"/>
       <c r="AK40" s="36"/>
-      <c r="AL40" s="36"/>
+      <c r="AL40" s="123"/>
       <c r="AM40" s="36"/>
       <c r="AN40" s="36"/>
       <c r="AO40" s="37"/>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="B41" s="36"/>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
+      <c r="E41" s="123"/>
       <c r="F41" s="9"/>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
+      <c r="I41" s="36">
+        <v>300000</v>
+      </c>
       <c r="J41" s="36"/>
       <c r="K41" s="36"/>
       <c r="L41" s="36"/>
       <c r="M41" s="36"/>
       <c r="N41" s="36"/>
       <c r="O41" s="36"/>
-      <c r="P41" s="36">
-        <v>50000</v>
-      </c>
+      <c r="P41" s="36"/>
       <c r="Q41" s="36"/>
       <c r="R41" s="36"/>
       <c r="S41" s="36"/>
@@ -15773,774 +15798,770 @@
       <c r="AE41" s="36"/>
       <c r="AF41" s="36"/>
       <c r="AG41" s="36"/>
-      <c r="AH41" s="36"/>
+      <c r="AH41" s="123"/>
       <c r="AI41" s="36"/>
-      <c r="AJ41" s="36"/>
+      <c r="AJ41" s="123"/>
       <c r="AK41" s="36"/>
-      <c r="AL41" s="36"/>
+      <c r="AL41" s="123"/>
       <c r="AM41" s="36"/>
       <c r="AN41" s="36"/>
       <c r="AO41" s="37"/>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="36">
-        <v>50000</v>
-      </c>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="36">
-        <v>50000</v>
-      </c>
-      <c r="R42" s="36"/>
-      <c r="S42" s="36"/>
-      <c r="T42" s="36"/>
-      <c r="U42" s="36"/>
-      <c r="V42" s="36"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="36"/>
-      <c r="Z42" s="36"/>
-      <c r="AA42" s="36"/>
-      <c r="AB42" s="36"/>
-      <c r="AC42" s="36"/>
-      <c r="AD42" s="36"/>
-      <c r="AE42" s="36"/>
-      <c r="AF42" s="36"/>
-      <c r="AG42" s="36"/>
-      <c r="AH42" s="36"/>
-      <c r="AI42" s="36"/>
-      <c r="AJ42" s="36"/>
-      <c r="AK42" s="36"/>
-      <c r="AL42" s="36"/>
-      <c r="AM42" s="36"/>
-      <c r="AN42" s="36"/>
-      <c r="AO42" s="37"/>
+      <c r="A42" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="122"/>
+      <c r="C42" s="122"/>
+      <c r="D42" s="122"/>
+      <c r="E42" s="124"/>
+      <c r="F42" s="117"/>
+      <c r="G42" s="122"/>
+      <c r="H42" s="122"/>
+      <c r="I42" s="122"/>
+      <c r="J42" s="122"/>
+      <c r="K42" s="122"/>
+      <c r="L42" s="122"/>
+      <c r="M42" s="122"/>
+      <c r="N42" s="122"/>
+      <c r="O42" s="122"/>
+      <c r="P42" s="122"/>
+      <c r="Q42" s="122"/>
+      <c r="R42" s="122"/>
+      <c r="S42" s="122"/>
+      <c r="T42" s="122"/>
+      <c r="U42" s="122"/>
+      <c r="V42" s="122">
+        <v>100000</v>
+      </c>
+      <c r="W42" s="122">
+        <v>300000</v>
+      </c>
+      <c r="X42" s="122"/>
+      <c r="Y42" s="122"/>
+      <c r="Z42" s="122"/>
+      <c r="AA42" s="122"/>
+      <c r="AB42" s="122"/>
+      <c r="AC42" s="122"/>
+      <c r="AD42" s="122"/>
+      <c r="AE42" s="122"/>
+      <c r="AF42" s="122"/>
+      <c r="AG42" s="122"/>
+      <c r="AH42" s="124"/>
+      <c r="AI42" s="122"/>
+      <c r="AJ42" s="124"/>
+      <c r="AK42" s="122"/>
+      <c r="AL42" s="124"/>
+      <c r="AM42" s="122"/>
+      <c r="AN42" s="122"/>
+      <c r="AO42" s="53"/>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="43"/>
-      <c r="N43" s="43"/>
-      <c r="O43" s="43"/>
-      <c r="P43" s="43"/>
-      <c r="Q43" s="43"/>
-      <c r="R43" s="43"/>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
-      <c r="U43" s="43">
-        <v>100000</v>
-      </c>
-      <c r="V43" s="43"/>
-      <c r="W43" s="43"/>
-      <c r="X43" s="43"/>
-      <c r="Y43" s="43"/>
-      <c r="Z43" s="43"/>
-      <c r="AA43" s="43"/>
-      <c r="AB43" s="43"/>
-      <c r="AC43" s="43"/>
-      <c r="AD43" s="43"/>
-      <c r="AE43" s="43"/>
-      <c r="AF43" s="43"/>
-      <c r="AG43" s="43"/>
-      <c r="AH43" s="43"/>
-      <c r="AI43" s="43"/>
-      <c r="AJ43" s="43"/>
-      <c r="AK43" s="43"/>
-      <c r="AL43" s="43"/>
-      <c r="AM43" s="43"/>
-      <c r="AN43" s="43"/>
+        <v>112</v>
+      </c>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="36">
+        <v>50000</v>
+      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="O43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="36"/>
+      <c r="R43" s="36"/>
+      <c r="S43" s="36"/>
+      <c r="T43" s="36"/>
+      <c r="U43" s="36"/>
+      <c r="V43" s="36"/>
+      <c r="W43" s="36"/>
+      <c r="X43" s="36"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="36"/>
+      <c r="AA43" s="36"/>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="36"/>
+      <c r="AD43" s="36"/>
+      <c r="AE43" s="36"/>
+      <c r="AF43" s="36"/>
+      <c r="AG43" s="36"/>
+      <c r="AH43" s="123"/>
+      <c r="AI43" s="36"/>
+      <c r="AJ43" s="123"/>
+      <c r="AK43" s="36"/>
+      <c r="AL43" s="123"/>
+      <c r="AM43" s="36"/>
+      <c r="AN43" s="36"/>
       <c r="AO43" s="37"/>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
+        <v>3</v>
+      </c>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="123"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-      <c r="N44" s="43"/>
-      <c r="O44" s="43"/>
-      <c r="P44" s="43"/>
-      <c r="Q44" s="43"/>
-      <c r="R44" s="43"/>
-      <c r="S44" s="43"/>
-      <c r="T44" s="43">
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36">
         <v>100000</v>
       </c>
-      <c r="U44" s="43"/>
-      <c r="V44" s="43"/>
-      <c r="W44" s="43"/>
-      <c r="X44" s="43"/>
-      <c r="Y44" s="43"/>
-      <c r="Z44" s="43"/>
-      <c r="AA44" s="43"/>
-      <c r="AB44" s="43"/>
-      <c r="AC44" s="43"/>
-      <c r="AD44" s="43"/>
-      <c r="AE44" s="43"/>
-      <c r="AF44" s="43"/>
-      <c r="AG44" s="43"/>
-      <c r="AH44" s="43"/>
-      <c r="AI44" s="43"/>
-      <c r="AJ44" s="43"/>
-      <c r="AK44" s="43"/>
-      <c r="AL44" s="43"/>
-      <c r="AM44" s="43"/>
-      <c r="AN44" s="43"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
+      <c r="O44" s="36"/>
+      <c r="P44" s="36"/>
+      <c r="Q44" s="36"/>
+      <c r="R44" s="36"/>
+      <c r="S44" s="36"/>
+      <c r="T44" s="36"/>
+      <c r="U44" s="36"/>
+      <c r="V44" s="36"/>
+      <c r="W44" s="36"/>
+      <c r="X44" s="36"/>
+      <c r="Y44" s="36"/>
+      <c r="Z44" s="36"/>
+      <c r="AA44" s="36"/>
+      <c r="AB44" s="36"/>
+      <c r="AC44" s="36"/>
+      <c r="AD44" s="36"/>
+      <c r="AE44" s="36"/>
+      <c r="AF44" s="36"/>
+      <c r="AG44" s="36"/>
+      <c r="AH44" s="123"/>
+      <c r="AI44" s="36"/>
+      <c r="AJ44" s="123"/>
+      <c r="AK44" s="36"/>
+      <c r="AL44" s="123"/>
+      <c r="AM44" s="36"/>
+      <c r="AN44" s="36"/>
       <c r="AO44" s="37"/>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
+        <v>4</v>
+      </c>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="123"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="43"/>
-      <c r="O45" s="43"/>
-      <c r="P45" s="43"/>
-      <c r="Q45" s="43"/>
-      <c r="R45" s="43"/>
-      <c r="S45" s="43"/>
-      <c r="T45" s="43"/>
-      <c r="U45" s="43"/>
-      <c r="V45" s="43"/>
-      <c r="W45" s="43">
-        <v>100000</v>
-      </c>
-      <c r="X45" s="43"/>
-      <c r="Y45" s="43"/>
-      <c r="Z45" s="43"/>
-      <c r="AA45" s="43"/>
-      <c r="AB45" s="43"/>
-      <c r="AC45" s="43"/>
-      <c r="AD45" s="43"/>
-      <c r="AE45" s="43"/>
-      <c r="AF45" s="43"/>
-      <c r="AG45" s="43"/>
-      <c r="AH45" s="43"/>
-      <c r="AI45" s="43"/>
-      <c r="AJ45" s="43"/>
-      <c r="AK45" s="43"/>
-      <c r="AL45" s="43"/>
-      <c r="AM45" s="43"/>
-      <c r="AN45" s="43"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36">
+        <v>75000</v>
+      </c>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="36"/>
+      <c r="Q45" s="36"/>
+      <c r="R45" s="36"/>
+      <c r="S45" s="36"/>
+      <c r="T45" s="36"/>
+      <c r="U45" s="36"/>
+      <c r="V45" s="36"/>
+      <c r="W45" s="36"/>
+      <c r="X45" s="36"/>
+      <c r="Y45" s="36"/>
+      <c r="Z45" s="36"/>
+      <c r="AA45" s="36"/>
+      <c r="AB45" s="36"/>
+      <c r="AC45" s="36"/>
+      <c r="AD45" s="36"/>
+      <c r="AE45" s="36"/>
+      <c r="AF45" s="36"/>
+      <c r="AG45" s="36"/>
+      <c r="AH45" s="123"/>
+      <c r="AI45" s="36"/>
+      <c r="AJ45" s="123"/>
+      <c r="AK45" s="36"/>
+      <c r="AL45" s="123"/>
+      <c r="AM45" s="36"/>
+      <c r="AN45" s="36"/>
       <c r="AO45" s="37"/>
     </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
+        <v>104</v>
+      </c>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="123"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="43"/>
-      <c r="P46" s="43"/>
-      <c r="Q46" s="43"/>
-      <c r="R46" s="43"/>
-      <c r="S46" s="43"/>
-      <c r="T46" s="43"/>
-      <c r="U46" s="43"/>
-      <c r="V46" s="43"/>
-      <c r="W46" s="43"/>
-      <c r="X46" s="43"/>
-      <c r="Y46" s="43"/>
-      <c r="Z46" s="43">
-        <v>100000</v>
-      </c>
-      <c r="AA46" s="43"/>
-      <c r="AB46" s="43"/>
-      <c r="AC46" s="43"/>
-      <c r="AD46" s="43"/>
-      <c r="AE46" s="43"/>
-      <c r="AF46" s="43"/>
-      <c r="AG46" s="43"/>
-      <c r="AH46" s="43"/>
-      <c r="AI46" s="43"/>
-      <c r="AJ46" s="43"/>
-      <c r="AK46" s="43"/>
-      <c r="AL46" s="43"/>
-      <c r="AM46" s="43"/>
-      <c r="AN46" s="43"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="36"/>
+      <c r="P46" s="36">
+        <v>50000</v>
+      </c>
+      <c r="Q46" s="36"/>
+      <c r="R46" s="36"/>
+      <c r="S46" s="36"/>
+      <c r="T46" s="36"/>
+      <c r="U46" s="36"/>
+      <c r="V46" s="36"/>
+      <c r="W46" s="36"/>
+      <c r="X46" s="36"/>
+      <c r="Y46" s="36"/>
+      <c r="Z46" s="36"/>
+      <c r="AA46" s="36"/>
+      <c r="AB46" s="36"/>
+      <c r="AC46" s="36"/>
+      <c r="AD46" s="36"/>
+      <c r="AE46" s="36"/>
+      <c r="AF46" s="36"/>
+      <c r="AG46" s="36"/>
+      <c r="AH46" s="123"/>
+      <c r="AI46" s="36"/>
+      <c r="AJ46" s="123"/>
+      <c r="AK46" s="36"/>
+      <c r="AL46" s="123"/>
+      <c r="AM46" s="36"/>
+      <c r="AN46" s="36"/>
       <c r="AO46" s="37"/>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
+        <v>105</v>
+      </c>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="123"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="43"/>
-      <c r="S47" s="43"/>
-      <c r="T47" s="43"/>
-      <c r="U47" s="43"/>
-      <c r="V47" s="43"/>
-      <c r="W47" s="43"/>
-      <c r="X47" s="43">
-        <v>100000</v>
-      </c>
-      <c r="Y47" s="43"/>
-      <c r="Z47" s="43"/>
-      <c r="AA47" s="43"/>
-      <c r="AB47" s="43"/>
-      <c r="AC47" s="43"/>
-      <c r="AD47" s="43"/>
-      <c r="AE47" s="43"/>
-      <c r="AF47" s="43"/>
-      <c r="AG47" s="43"/>
-      <c r="AH47" s="43"/>
-      <c r="AI47" s="43"/>
-      <c r="AJ47" s="43"/>
-      <c r="AK47" s="43"/>
-      <c r="AL47" s="43"/>
-      <c r="AM47" s="43"/>
-      <c r="AN47" s="43"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="36">
+        <v>50000</v>
+      </c>
+      <c r="P47" s="36"/>
+      <c r="Q47" s="36">
+        <v>50000</v>
+      </c>
+      <c r="R47" s="36"/>
+      <c r="S47" s="36"/>
+      <c r="T47" s="36"/>
+      <c r="U47" s="36"/>
+      <c r="V47" s="36"/>
+      <c r="W47" s="36"/>
+      <c r="X47" s="36"/>
+      <c r="Y47" s="36"/>
+      <c r="Z47" s="36"/>
+      <c r="AA47" s="36"/>
+      <c r="AB47" s="36"/>
+      <c r="AC47" s="36"/>
+      <c r="AD47" s="36"/>
+      <c r="AE47" s="36"/>
+      <c r="AF47" s="36"/>
+      <c r="AG47" s="36"/>
+      <c r="AH47" s="123"/>
+      <c r="AI47" s="36"/>
+      <c r="AJ47" s="123"/>
+      <c r="AK47" s="36"/>
+      <c r="AL47" s="123"/>
+      <c r="AM47" s="36"/>
+      <c r="AN47" s="36"/>
       <c r="AO47" s="37"/>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
+        <v>106</v>
+      </c>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="123"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="43"/>
-      <c r="N48" s="43"/>
-      <c r="O48" s="43"/>
-      <c r="P48" s="43"/>
-      <c r="Q48" s="43"/>
-      <c r="R48" s="43"/>
-      <c r="S48" s="43"/>
-      <c r="T48" s="43"/>
-      <c r="U48" s="43"/>
-      <c r="V48" s="43"/>
-      <c r="W48" s="43"/>
-      <c r="X48" s="43"/>
-      <c r="Y48" s="43"/>
-      <c r="Z48" s="43"/>
-      <c r="AA48" s="43"/>
-      <c r="AB48" s="43"/>
-      <c r="AC48" s="43"/>
-      <c r="AD48" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AE48" s="43"/>
-      <c r="AF48" s="43"/>
-      <c r="AG48" s="43"/>
-      <c r="AH48" s="43"/>
-      <c r="AI48" s="43"/>
-      <c r="AJ48" s="43"/>
-      <c r="AK48" s="43"/>
-      <c r="AL48" s="43"/>
-      <c r="AM48" s="43"/>
-      <c r="AN48" s="43"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="36"/>
+      <c r="O48" s="36"/>
+      <c r="P48" s="36"/>
+      <c r="Q48" s="36"/>
+      <c r="R48" s="36"/>
+      <c r="S48" s="36"/>
+      <c r="T48" s="36"/>
+      <c r="U48" s="36">
+        <v>100000</v>
+      </c>
+      <c r="V48" s="36"/>
+      <c r="W48" s="36"/>
+      <c r="X48" s="36"/>
+      <c r="Y48" s="36"/>
+      <c r="Z48" s="36"/>
+      <c r="AA48" s="36"/>
+      <c r="AB48" s="36"/>
+      <c r="AC48" s="36"/>
+      <c r="AD48" s="36"/>
+      <c r="AE48" s="36"/>
+      <c r="AF48" s="36"/>
+      <c r="AG48" s="36"/>
+      <c r="AH48" s="123"/>
+      <c r="AI48" s="36"/>
+      <c r="AJ48" s="123"/>
+      <c r="AK48" s="36"/>
+      <c r="AL48" s="123"/>
+      <c r="AM48" s="36"/>
+      <c r="AN48" s="36"/>
       <c r="AO48" s="37"/>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
+        <v>107</v>
+      </c>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="123"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
-      <c r="P49" s="43"/>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="43"/>
-      <c r="S49" s="43"/>
-      <c r="T49" s="43"/>
-      <c r="U49" s="43"/>
-      <c r="V49" s="43"/>
-      <c r="W49" s="43"/>
-      <c r="X49" s="43"/>
-      <c r="Y49" s="43"/>
-      <c r="Z49" s="43"/>
-      <c r="AA49" s="43"/>
-      <c r="AB49" s="43"/>
-      <c r="AC49" s="43"/>
-      <c r="AD49" s="43"/>
-      <c r="AE49" s="43"/>
-      <c r="AF49" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AG49" s="43"/>
-      <c r="AH49" s="43"/>
-      <c r="AI49" s="43"/>
-      <c r="AJ49" s="43"/>
-      <c r="AK49" s="43"/>
-      <c r="AL49" s="43"/>
-      <c r="AM49" s="43"/>
-      <c r="AN49" s="43"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="36"/>
+      <c r="N49" s="36"/>
+      <c r="O49" s="36"/>
+      <c r="P49" s="36"/>
+      <c r="Q49" s="36"/>
+      <c r="R49" s="36"/>
+      <c r="S49" s="36"/>
+      <c r="T49" s="36">
+        <v>100000</v>
+      </c>
+      <c r="U49" s="36"/>
+      <c r="V49" s="36"/>
+      <c r="W49" s="36"/>
+      <c r="X49" s="36"/>
+      <c r="Y49" s="36"/>
+      <c r="Z49" s="36"/>
+      <c r="AA49" s="36"/>
+      <c r="AB49" s="36"/>
+      <c r="AC49" s="36"/>
+      <c r="AD49" s="36"/>
+      <c r="AE49" s="36"/>
+      <c r="AF49" s="36"/>
+      <c r="AG49" s="36"/>
+      <c r="AH49" s="123"/>
+      <c r="AI49" s="36"/>
+      <c r="AJ49" s="123"/>
+      <c r="AK49" s="36"/>
+      <c r="AL49" s="123"/>
+      <c r="AM49" s="36"/>
+      <c r="AN49" s="36"/>
       <c r="AO49" s="37"/>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
+        <v>108</v>
+      </c>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="123"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-      <c r="M50" s="43"/>
-      <c r="N50" s="43"/>
-      <c r="O50" s="43"/>
-      <c r="P50" s="43"/>
-      <c r="Q50" s="43"/>
-      <c r="R50" s="43"/>
-      <c r="S50" s="43"/>
-      <c r="T50" s="43"/>
-      <c r="U50" s="43"/>
-      <c r="V50" s="43"/>
-      <c r="W50" s="43"/>
-      <c r="X50" s="43"/>
-      <c r="Y50" s="43"/>
-      <c r="Z50" s="43"/>
-      <c r="AA50" s="43"/>
-      <c r="AB50" s="43"/>
-      <c r="AC50" s="43"/>
-      <c r="AD50" s="43"/>
-      <c r="AE50" s="43"/>
-      <c r="AF50" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AG50" s="43"/>
-      <c r="AH50" s="43"/>
-      <c r="AI50" s="43"/>
-      <c r="AJ50" s="43"/>
-      <c r="AK50" s="43"/>
-      <c r="AL50" s="43"/>
-      <c r="AM50" s="43"/>
-      <c r="AN50" s="43"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="36"/>
+      <c r="O50" s="36"/>
+      <c r="P50" s="36"/>
+      <c r="Q50" s="36"/>
+      <c r="R50" s="36"/>
+      <c r="S50" s="36"/>
+      <c r="T50" s="36"/>
+      <c r="U50" s="36"/>
+      <c r="V50" s="36"/>
+      <c r="W50" s="36">
+        <v>100000</v>
+      </c>
+      <c r="X50" s="36"/>
+      <c r="Y50" s="36"/>
+      <c r="Z50" s="36"/>
+      <c r="AA50" s="36"/>
+      <c r="AB50" s="36"/>
+      <c r="AC50" s="36"/>
+      <c r="AD50" s="36"/>
+      <c r="AE50" s="36"/>
+      <c r="AF50" s="36"/>
+      <c r="AG50" s="36"/>
+      <c r="AH50" s="123"/>
+      <c r="AI50" s="36"/>
+      <c r="AJ50" s="123"/>
+      <c r="AK50" s="36"/>
+      <c r="AL50" s="123"/>
+      <c r="AM50" s="36"/>
+      <c r="AN50" s="36"/>
       <c r="AO50" s="37"/>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
+        <v>109</v>
+      </c>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="123"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="43"/>
-      <c r="N51" s="43"/>
-      <c r="O51" s="43"/>
-      <c r="P51" s="43"/>
-      <c r="Q51" s="43"/>
-      <c r="R51" s="43"/>
-      <c r="S51" s="43"/>
-      <c r="T51" s="43"/>
-      <c r="U51" s="43"/>
-      <c r="V51" s="43"/>
-      <c r="W51" s="43"/>
-      <c r="X51" s="43"/>
-      <c r="Y51" s="43"/>
-      <c r="Z51" s="43"/>
-      <c r="AA51" s="43"/>
-      <c r="AB51" s="43"/>
-      <c r="AC51" s="43"/>
-      <c r="AD51" s="43"/>
-      <c r="AE51" s="43"/>
-      <c r="AF51" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AG51" s="43"/>
-      <c r="AH51" s="43"/>
-      <c r="AI51" s="43"/>
-      <c r="AJ51" s="43"/>
-      <c r="AK51" s="43"/>
-      <c r="AL51" s="43"/>
-      <c r="AM51" s="43"/>
-      <c r="AN51" s="43"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
+      <c r="N51" s="36"/>
+      <c r="O51" s="36"/>
+      <c r="P51" s="36"/>
+      <c r="Q51" s="36"/>
+      <c r="R51" s="36"/>
+      <c r="S51" s="36"/>
+      <c r="T51" s="36"/>
+      <c r="U51" s="36"/>
+      <c r="V51" s="36"/>
+      <c r="W51" s="36"/>
+      <c r="X51" s="36"/>
+      <c r="Y51" s="36"/>
+      <c r="Z51" s="36">
+        <v>100000</v>
+      </c>
+      <c r="AA51" s="36"/>
+      <c r="AB51" s="36"/>
+      <c r="AC51" s="36"/>
+      <c r="AD51" s="36"/>
+      <c r="AE51" s="36"/>
+      <c r="AF51" s="36"/>
+      <c r="AG51" s="36"/>
+      <c r="AH51" s="123"/>
+      <c r="AI51" s="36"/>
+      <c r="AJ51" s="123"/>
+      <c r="AK51" s="36"/>
+      <c r="AL51" s="123"/>
+      <c r="AM51" s="36"/>
+      <c r="AN51" s="36"/>
       <c r="AO51" s="37"/>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
+        <v>110</v>
+      </c>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="123"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
-      <c r="N52" s="43"/>
-      <c r="O52" s="43"/>
-      <c r="P52" s="43"/>
-      <c r="Q52" s="43"/>
-      <c r="R52" s="43"/>
-      <c r="S52" s="43"/>
-      <c r="T52" s="43"/>
-      <c r="U52" s="43"/>
-      <c r="V52" s="43"/>
-      <c r="W52" s="43"/>
-      <c r="X52" s="43"/>
-      <c r="Y52" s="43"/>
-      <c r="Z52" s="43"/>
-      <c r="AA52" s="43"/>
-      <c r="AB52" s="43"/>
-      <c r="AC52" s="43">
-        <v>50000</v>
-      </c>
-      <c r="AD52" s="43"/>
-      <c r="AE52" s="43"/>
-      <c r="AF52" s="43"/>
-      <c r="AG52" s="43"/>
-      <c r="AH52" s="43"/>
-      <c r="AI52" s="43"/>
-      <c r="AJ52" s="43"/>
-      <c r="AK52" s="43"/>
-      <c r="AL52" s="43"/>
-      <c r="AM52" s="43"/>
-      <c r="AN52" s="43"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="36"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="36"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="36"/>
+      <c r="T52" s="36"/>
+      <c r="U52" s="36"/>
+      <c r="V52" s="36"/>
+      <c r="W52" s="36"/>
+      <c r="X52" s="36">
+        <v>100000</v>
+      </c>
+      <c r="Y52" s="36"/>
+      <c r="Z52" s="36"/>
+      <c r="AA52" s="36"/>
+      <c r="AB52" s="36"/>
+      <c r="AC52" s="36"/>
+      <c r="AD52" s="36"/>
+      <c r="AE52" s="36"/>
+      <c r="AF52" s="36"/>
+      <c r="AG52" s="36"/>
+      <c r="AH52" s="123"/>
+      <c r="AI52" s="36"/>
+      <c r="AJ52" s="123"/>
+      <c r="AK52" s="36"/>
+      <c r="AL52" s="123"/>
+      <c r="AM52" s="36"/>
+      <c r="AN52" s="36"/>
       <c r="AO52" s="37"/>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="36">
-        <v>150000</v>
-      </c>
-      <c r="C53" s="36">
-        <v>150000</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
       <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
+      <c r="E53" s="123"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="43"/>
-      <c r="O53" s="43"/>
-      <c r="P53" s="43"/>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
-      <c r="S53" s="43"/>
-      <c r="T53" s="43"/>
-      <c r="U53" s="43"/>
-      <c r="V53" s="43"/>
-      <c r="W53" s="43"/>
-      <c r="X53" s="43"/>
-      <c r="Y53" s="43"/>
-      <c r="Z53" s="43"/>
-      <c r="AA53" s="43"/>
-      <c r="AB53" s="43"/>
-      <c r="AC53" s="43"/>
-      <c r="AD53" s="43"/>
-      <c r="AE53" s="43"/>
-      <c r="AF53" s="43"/>
-      <c r="AG53" s="43"/>
-      <c r="AH53" s="43"/>
-      <c r="AI53" s="36">
-        <v>300000</v>
-      </c>
-      <c r="AJ53" s="43"/>
-      <c r="AK53" s="43"/>
-      <c r="AL53" s="43"/>
-      <c r="AM53" s="43"/>
-      <c r="AN53" s="43"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="36"/>
+      <c r="N53" s="36"/>
+      <c r="O53" s="36"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="36"/>
+      <c r="R53" s="36"/>
+      <c r="S53" s="36"/>
+      <c r="T53" s="36"/>
+      <c r="U53" s="36"/>
+      <c r="V53" s="36"/>
+      <c r="W53" s="36"/>
+      <c r="X53" s="36"/>
+      <c r="Y53" s="36"/>
+      <c r="Z53" s="36"/>
+      <c r="AA53" s="36"/>
+      <c r="AB53" s="36"/>
+      <c r="AC53" s="36"/>
+      <c r="AD53" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AE53" s="36"/>
+      <c r="AF53" s="36"/>
+      <c r="AG53" s="36"/>
+      <c r="AH53" s="123"/>
+      <c r="AI53" s="36"/>
+      <c r="AJ53" s="123"/>
+      <c r="AK53" s="36"/>
+      <c r="AL53" s="123"/>
+      <c r="AM53" s="36"/>
+      <c r="AN53" s="36"/>
       <c r="AO53" s="37"/>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
-        <v>287</v>
+        <v>113</v>
       </c>
       <c r="B54" s="36"/>
       <c r="C54" s="36"/>
-      <c r="D54" s="36">
-        <v>150000</v>
-      </c>
-      <c r="E54" s="36">
-        <v>150000</v>
-      </c>
+      <c r="D54" s="36"/>
+      <c r="E54" s="123"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="43"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="43"/>
-      <c r="O54" s="43"/>
-      <c r="P54" s="43"/>
-      <c r="Q54" s="43"/>
-      <c r="R54" s="43"/>
-      <c r="S54" s="43"/>
-      <c r="T54" s="43"/>
-      <c r="U54" s="43"/>
-      <c r="V54" s="43"/>
-      <c r="W54" s="43"/>
-      <c r="X54" s="43"/>
-      <c r="Y54" s="43"/>
-      <c r="Z54" s="43"/>
-      <c r="AA54" s="43"/>
-      <c r="AB54" s="43"/>
-      <c r="AC54" s="43"/>
-      <c r="AD54" s="43"/>
-      <c r="AE54" s="43"/>
-      <c r="AF54" s="43"/>
-      <c r="AG54" s="43"/>
-      <c r="AH54" s="43"/>
-      <c r="AI54" s="43"/>
-      <c r="AJ54" s="36">
-        <v>300000</v>
-      </c>
-      <c r="AK54" s="43"/>
-      <c r="AL54" s="43"/>
-      <c r="AM54" s="43"/>
-      <c r="AN54" s="43"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="36"/>
+      <c r="M54" s="36"/>
+      <c r="N54" s="36"/>
+      <c r="O54" s="36"/>
+      <c r="P54" s="36"/>
+      <c r="Q54" s="36"/>
+      <c r="R54" s="36"/>
+      <c r="S54" s="36"/>
+      <c r="T54" s="36"/>
+      <c r="U54" s="36"/>
+      <c r="V54" s="36"/>
+      <c r="W54" s="36"/>
+      <c r="X54" s="36"/>
+      <c r="Y54" s="36"/>
+      <c r="Z54" s="36"/>
+      <c r="AA54" s="36"/>
+      <c r="AB54" s="36"/>
+      <c r="AC54" s="36"/>
+      <c r="AD54" s="36"/>
+      <c r="AE54" s="36"/>
+      <c r="AF54" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AG54" s="36"/>
+      <c r="AH54" s="123"/>
+      <c r="AI54" s="36"/>
+      <c r="AJ54" s="123"/>
+      <c r="AK54" s="36"/>
+      <c r="AL54" s="123"/>
+      <c r="AM54" s="36"/>
+      <c r="AN54" s="36"/>
       <c r="AO54" s="37"/>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="9">
-        <v>100000</v>
-      </c>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="43"/>
-      <c r="P55" s="43"/>
-      <c r="Q55" s="43"/>
-      <c r="R55" s="43"/>
-      <c r="S55" s="43"/>
-      <c r="T55" s="43"/>
-      <c r="U55" s="43"/>
-      <c r="V55" s="43"/>
-      <c r="W55" s="43"/>
-      <c r="X55" s="43"/>
-      <c r="Y55" s="43"/>
-      <c r="Z55" s="43"/>
-      <c r="AA55" s="43"/>
-      <c r="AB55" s="43"/>
-      <c r="AC55" s="43"/>
-      <c r="AD55" s="43"/>
-      <c r="AE55" s="43"/>
-      <c r="AF55" s="43"/>
-      <c r="AG55" s="43"/>
-      <c r="AH55" s="43"/>
-      <c r="AI55" s="43"/>
-      <c r="AJ55" s="43"/>
-      <c r="AK55" s="43"/>
-      <c r="AL55" s="43"/>
-      <c r="AM55" s="43"/>
-      <c r="AN55" s="43"/>
+        <v>114</v>
+      </c>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="36"/>
+      <c r="M55" s="36"/>
+      <c r="N55" s="36"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="36"/>
+      <c r="Q55" s="36"/>
+      <c r="R55" s="36"/>
+      <c r="S55" s="36"/>
+      <c r="T55" s="36"/>
+      <c r="U55" s="36"/>
+      <c r="V55" s="36"/>
+      <c r="W55" s="36"/>
+      <c r="X55" s="36"/>
+      <c r="Y55" s="36"/>
+      <c r="Z55" s="36"/>
+      <c r="AA55" s="36"/>
+      <c r="AB55" s="36"/>
+      <c r="AC55" s="36"/>
+      <c r="AD55" s="36"/>
+      <c r="AE55" s="36"/>
+      <c r="AF55" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AG55" s="36"/>
+      <c r="AH55" s="123"/>
+      <c r="AI55" s="36"/>
+      <c r="AJ55" s="123"/>
+      <c r="AK55" s="36"/>
+      <c r="AL55" s="123"/>
+      <c r="AM55" s="36"/>
+      <c r="AN55" s="36"/>
       <c r="AO55" s="37"/>
     </row>
     <row r="56" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
+        <v>115</v>
+      </c>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="123"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
-      <c r="M56" s="43"/>
-      <c r="N56" s="43"/>
-      <c r="O56" s="43"/>
-      <c r="P56" s="43"/>
-      <c r="Q56" s="43"/>
-      <c r="R56" s="43"/>
-      <c r="S56" s="43"/>
-      <c r="T56" s="43"/>
-      <c r="U56" s="43"/>
-      <c r="V56" s="43"/>
-      <c r="W56" s="43"/>
-      <c r="X56" s="43"/>
-      <c r="Y56" s="43"/>
-      <c r="Z56" s="43"/>
-      <c r="AA56" s="43"/>
-      <c r="AB56" s="43"/>
-      <c r="AC56" s="43"/>
-      <c r="AD56" s="43"/>
-      <c r="AE56" s="43"/>
-      <c r="AF56" s="43"/>
-      <c r="AG56" s="43"/>
-      <c r="AH56" s="43"/>
-      <c r="AI56" s="43"/>
-      <c r="AJ56" s="43"/>
-      <c r="AK56" s="43"/>
-      <c r="AL56" s="43"/>
-      <c r="AM56" s="43"/>
-      <c r="AN56" s="43"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="36"/>
+      <c r="N56" s="36"/>
+      <c r="O56" s="36"/>
+      <c r="P56" s="36"/>
+      <c r="Q56" s="36"/>
+      <c r="R56" s="36"/>
+      <c r="S56" s="36"/>
+      <c r="T56" s="36"/>
+      <c r="U56" s="36"/>
+      <c r="V56" s="36"/>
+      <c r="W56" s="36"/>
+      <c r="X56" s="36"/>
+      <c r="Y56" s="36"/>
+      <c r="Z56" s="36"/>
+      <c r="AA56" s="36"/>
+      <c r="AB56" s="36"/>
+      <c r="AC56" s="36"/>
+      <c r="AD56" s="36"/>
+      <c r="AE56" s="36"/>
+      <c r="AF56" s="36">
+        <v>50000</v>
+      </c>
+      <c r="AG56" s="36"/>
+      <c r="AH56" s="123"/>
+      <c r="AI56" s="36"/>
+      <c r="AJ56" s="123"/>
+      <c r="AK56" s="36"/>
+      <c r="AL56" s="123"/>
+      <c r="AM56" s="36"/>
+      <c r="AN56" s="36"/>
       <c r="AO56" s="37"/>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="43"/>
-      <c r="L57" s="43"/>
-      <c r="M57" s="43"/>
-      <c r="N57" s="43"/>
-      <c r="O57" s="43"/>
-      <c r="P57" s="43"/>
-      <c r="Q57" s="43"/>
-      <c r="R57" s="43"/>
-      <c r="S57" s="43"/>
-      <c r="T57" s="43"/>
-      <c r="U57" s="43"/>
-      <c r="V57" s="43"/>
-      <c r="W57" s="43">
-        <v>300000</v>
-      </c>
-      <c r="X57" s="43"/>
-      <c r="Y57" s="43"/>
-      <c r="Z57" s="43"/>
-      <c r="AA57" s="43"/>
-      <c r="AB57" s="43"/>
-      <c r="AC57" s="43"/>
-      <c r="AD57" s="43"/>
-      <c r="AE57" s="43"/>
-      <c r="AF57" s="43"/>
-      <c r="AG57" s="43"/>
-      <c r="AH57" s="43"/>
-      <c r="AI57" s="43"/>
-      <c r="AJ57" s="43"/>
-      <c r="AK57" s="43"/>
-      <c r="AL57" s="43"/>
-      <c r="AM57" s="43"/>
-      <c r="AN57" s="43"/>
-      <c r="AO57" s="37"/>
+    <row r="57" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="125"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38"/>
+      <c r="M57" s="38"/>
+      <c r="N57" s="38"/>
+      <c r="O57" s="38"/>
+      <c r="P57" s="38"/>
+      <c r="Q57" s="38"/>
+      <c r="R57" s="38"/>
+      <c r="S57" s="38"/>
+      <c r="T57" s="38"/>
+      <c r="U57" s="38"/>
+      <c r="V57" s="38"/>
+      <c r="W57" s="38"/>
+      <c r="X57" s="38"/>
+      <c r="Y57" s="38"/>
+      <c r="Z57" s="38"/>
+      <c r="AA57" s="38"/>
+      <c r="AB57" s="38"/>
+      <c r="AC57" s="38">
+        <v>50000</v>
+      </c>
+      <c r="AD57" s="38"/>
+      <c r="AE57" s="38"/>
+      <c r="AF57" s="38"/>
+      <c r="AG57" s="38"/>
+      <c r="AH57" s="125"/>
+      <c r="AI57" s="38"/>
+      <c r="AJ57" s="125"/>
+      <c r="AK57" s="38"/>
+      <c r="AL57" s="125"/>
+      <c r="AM57" s="38"/>
+      <c r="AN57" s="38"/>
+      <c r="AO57" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -29178,7 +29199,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>